<commit_message>
Extremes module: initialized changes to functions to process and load the extremes data
</commit_message>
<xml_diff>
--- a/inst/extdata/extremes/extremes_config.xlsx
+++ b/inst/extdata/extremes/extremes_config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9002BBCD-34DF-4CC3-9303-AF285EF1BF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B04C17-C7AF-4455-BF2F-7B73916D67E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7005" yWindow="-30225" windowWidth="27555" windowHeight="18675" tabRatio="764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2865" yWindow="-25080" windowWidth="27555" windowHeight="18675" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="48" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="loc_coImpactTypes">co_impactTypes[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coImpactYears">co_impactYears[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coInputScenarioInfo">co_inputInfo[[#Headers],[row_id]]</definedName>
-    <definedName name="loc_colorLegend">controlTables!$C$16</definedName>
+    <definedName name="loc_colorLegend">controlTables!$C$14</definedName>
     <definedName name="loc_coModels">co_models[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coModelTypes">co_modelTypes[[#Headers],[row_id]]</definedName>
     <definedName name="loc_controlTOC">controlTables!$B$1</definedName>
@@ -35,8 +35,8 @@
     <definedName name="loc_coStates">co_impactYears[[#Headers],[row_id]]</definedName>
     <definedName name="loc_econMultipliers">co_econMultipliers[[#Headers],[row_id]]</definedName>
     <definedName name="num_gcms">MAX(co_models[row_id])</definedName>
-    <definedName name="SectorDropDown">controlTables!$D$21:$D$21</definedName>
-    <definedName name="SectorDropDown_1">controlTables!$D$21:$D$21</definedName>
+    <definedName name="SectorDropDown">controlTables!$D$19:$D$19</definedName>
+    <definedName name="SectorDropDown_1">controlTables!$D$19:$D$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -128,7 +128,7 @@
     <author>tc={A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}</author>
   </authors>
   <commentList>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{B1227AEC-55F2-4D4B-9D62-D8081C156293}">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{B1227AEC-55F2-4D4B-9D62-D8081C156293}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -136,7 +136,7 @@
     Boolean field -- indicates if sector is included in run of R script.</t>
       </text>
     </comment>
-    <comment ref="J20" authorId="1" shapeId="0" xr:uid="{492F094F-8801-4499-80C3-4610B2EB4C3B}">
+    <comment ref="J18" authorId="1" shapeId="0" xr:uid="{492F094F-8801-4499-80C3-4610B2EB4C3B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -144,7 +144,7 @@
     Boolean field -- indicates if sector has 2010 and 2090 impact esimates. Corresponds to impact year table below.</t>
       </text>
     </comment>
-    <comment ref="D25" authorId="2" shapeId="0" xr:uid="{40274E0A-9A04-480D-A5E8-2C38F8B3CAD3}">
+    <comment ref="D23" authorId="2" shapeId="0" xr:uid="{40274E0A-9A04-480D-A5E8-2C38F8B3CAD3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -152,7 +152,7 @@
     Empty values are replaced with "NA" in the R tool.</t>
       </text>
     </comment>
-    <comment ref="E32" authorId="3" shapeId="0" xr:uid="{61FF9366-C253-4143-8900-DE7FDB924463}">
+    <comment ref="E30" authorId="3" shapeId="0" xr:uid="{61FF9366-C253-4143-8900-DE7FDB924463}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -160,7 +160,7 @@
     No spaces in this ID!</t>
       </text>
     </comment>
-    <comment ref="F32" authorId="4" shapeId="0" xr:uid="{7C7D377F-2B53-48B7-807A-23CFCBC48B83}">
+    <comment ref="F30" authorId="4" shapeId="0" xr:uid="{7C7D377F-2B53-48B7-807A-23CFCBC48B83}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -168,7 +168,7 @@
     For sectors with multiple variants, one variant is considered the "primary" variant -- e.g., as used in when aggregating across sectors.</t>
       </text>
     </comment>
-    <comment ref="G32" authorId="5" shapeId="0" xr:uid="{3962DDEC-520D-4477-AB4D-6A758B04F9CC}">
+    <comment ref="G30" authorId="5" shapeId="0" xr:uid="{3962DDEC-520D-4477-AB4D-6A758B04F9CC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -176,7 +176,7 @@
     Numeric field -- indicates whether a sector should be included when aggregating over sectors. Sectors with a flag &gt;= 1 are generally included in aggregation. Flags &gt; 1 may have different treatments</t>
       </text>
     </comment>
-    <comment ref="F46" authorId="6" shapeId="0" xr:uid="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
+    <comment ref="F44" authorId="6" shapeId="0" xr:uid="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -184,7 +184,7 @@
     This field tracks whether the input scalar is a time series of scalars, or a single input used to calculate a trajectory of the scalar in R. "Dynamic" scalars are a full series; "constant" are a single value from which a series is calculated in the R script.</t>
       </text>
     </comment>
-    <comment ref="J62" authorId="7" shapeId="0" xr:uid="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
+    <comment ref="J60" authorId="7" shapeId="0" xr:uid="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -192,7 +192,7 @@
     Year when change and impacts are zero</t>
       </text>
     </comment>
-    <comment ref="L62" authorId="8" shapeId="0" xr:uid="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
+    <comment ref="L60" authorId="8" shapeId="0" xr:uid="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -200,7 +200,7 @@
     Maximum value to extrapolate to, for models that go up to the maximum output value.</t>
       </text>
     </comment>
-    <comment ref="D68" authorId="9" shapeId="0" xr:uid="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
+    <comment ref="D66" authorId="9" shapeId="0" xr:uid="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -208,7 +208,7 @@
     Max extrapolation temperature</t>
       </text>
     </comment>
-    <comment ref="J80" authorId="10" shapeId="0" xr:uid="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
+    <comment ref="J78" authorId="10" shapeId="0" xr:uid="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="344">
   <si>
     <t>CanESM2</t>
   </si>
@@ -702,9 +702,6 @@
   </si>
   <si>
     <t>Hard-coded value/included in model</t>
-  </si>
-  <si>
-    <t>Named constants</t>
   </si>
   <si>
     <t>Temperature and SLR-binning model types</t>
@@ -1299,9 +1296,6 @@
   </si>
   <si>
     <t>maxUnitValue</t>
-  </si>
-  <si>
-    <t>Info on SLR scalars past 2090</t>
   </si>
   <si>
     <t>Climate-Driven Changes in Air Quality</t>
@@ -6437,9 +6431,9 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C2AD6E-F129-4852-8BB5-5A249C234872}" name="co_variants" displayName="co_variants" ref="B32:I35" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B33:I35">
-    <sortCondition ref="C33:C35"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C2AD6E-F129-4852-8BB5-5A249C234872}" name="co_variants" displayName="co_variants" ref="B30:I33" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B31:I33">
+    <sortCondition ref="C31:C33"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1BCFA006-CF85-4F3A-AC79-60916A48ED39}" name="row_id" dataDxfId="53" totalsRowDxfId="52">
@@ -6463,7 +6457,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B55:E56" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B53:E54" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="36">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6477,7 +6471,7 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B80:J82" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B78:J80" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="30">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6498,8 +6492,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B99:F148" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="B99:F148" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B97:F146" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="B97:F146" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="20">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6608,10 +6602,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4FB08D13-3C4C-4BB6-9ED3-E44A55D938B0}" name="co_sectors" displayName="co_sectors" ref="B20:O21" totalsRowShown="0" headerRowDxfId="153" dataDxfId="151" headerRowBorderDxfId="152" tableBorderDxfId="150" totalsRowBorderDxfId="149">
-  <autoFilter ref="B20:O21" xr:uid="{4FB08D13-3C4C-4BB6-9ED3-E44A55D938B0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B21:O21">
-    <sortCondition ref="D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4FB08D13-3C4C-4BB6-9ED3-E44A55D938B0}" name="co_sectors" displayName="co_sectors" ref="B18:O19" totalsRowShown="0" headerRowDxfId="153" dataDxfId="151" headerRowBorderDxfId="152" tableBorderDxfId="150" totalsRowBorderDxfId="149">
+  <autoFilter ref="B18:O19" xr:uid="{4FB08D13-3C4C-4BB6-9ED3-E44A55D938B0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B19:O19">
+    <sortCondition ref="D19"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="14" xr3:uid="{60C3EA8F-72E0-495B-8B73-6D682443C60B}" name="row_id" dataDxfId="148" totalsRowDxfId="147">
@@ -6661,7 +6655,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{80839C52-E413-4982-A35C-46B477F75688}" name="co_modelTypes" displayName="co_modelTypes" ref="B62:L63" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{80839C52-E413-4982-A35C-46B477F75688}" name="co_modelTypes" displayName="co_modelTypes" ref="B60:L61" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{11DFD282-93A9-4795-9369-6627D14BB282}" name="row_id" dataDxfId="118">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6682,7 +6676,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBCED586-17E1-4B5C-A781-976D1E5A11BF}" name="co_regions" displayName="co_regions" ref="B87:D94" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBCED586-17E1-4B5C-A781-976D1E5A11BF}" name="co_regions" displayName="co_regions" ref="B85:D92" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{18599272-3810-42BA-A220-485AFB1D6807}" name="row_id" dataDxfId="105">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6697,7 +6691,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B68:F75" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B66:F73" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BF1485BD-F9FE-4F5B-9D9F-D9CB3D918F44}" name="row_id" dataDxfId="100">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6714,10 +6708,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FBBCD2EA-5DCC-406C-B109-DA7E04AF91C0}" name="co_impactYears" displayName="co_impactYears" ref="B25:F26" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
-  <autoFilter ref="B25:F26" xr:uid="{965CD6B2-887D-46C8-9D98-6C6AECBC7B1A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B26:F26">
-    <sortCondition ref="C26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FBBCD2EA-5DCC-406C-B109-DA7E04AF91C0}" name="co_impactYears" displayName="co_impactYears" ref="B23:F24" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+  <autoFilter ref="B23:F24" xr:uid="{965CD6B2-887D-46C8-9D98-6C6AECBC7B1A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B24:F24">
+    <sortCondition ref="C24"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{CDF8B6C0-3166-4A5F-954A-6DD921A48F0D}" name="row_id" dataDxfId="93" totalsRowDxfId="92">
@@ -6733,11 +6727,11 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BAD307D6-4C07-4313-AAAB-5A0F25B0CD27}" name="co_impactTypes" displayName="co_impactTypes" ref="B39:P41" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="B39:P41" xr:uid="{E446364F-959A-4BFF-80B5-CD65050C4865}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B40:P41">
-    <sortCondition ref="C40:C41"/>
-    <sortCondition ref="D40:D41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BAD307D6-4C07-4313-AAAB-5A0F25B0CD27}" name="co_impactTypes" displayName="co_impactTypes" ref="B37:P39" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="B37:P39" xr:uid="{E446364F-959A-4BFF-80B5-CD65050C4865}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B38:P39">
+    <sortCondition ref="C38:C39"/>
+    <sortCondition ref="D38:D39"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{3C0C87EC-3301-4189-A438-330FBC0C23CE}" name="row_id" dataDxfId="81">
@@ -6765,11 +6759,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B46:J50" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
-  <autoFilter ref="B46:J50" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B47:J50">
-    <sortCondition ref="E47:E50"/>
-    <sortCondition ref="C47:C50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B44:J48" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+  <autoFilter ref="B44:J48" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B45:J48">
+    <sortCondition ref="E45:E48"/>
+    <sortCondition ref="C45:C48"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="64">
@@ -7105,37 +7099,37 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E20" dT="2021-04-02T15:07:48.34" personId="{00000000-0000-0000-0000-000000000000}" id="{B1227AEC-55F2-4D4B-9D62-D8081C156293}">
+  <threadedComment ref="E18" dT="2021-04-02T15:07:48.34" personId="{00000000-0000-0000-0000-000000000000}" id="{B1227AEC-55F2-4D4B-9D62-D8081C156293}">
     <text>Boolean field -- indicates if sector is included in run of R script.</text>
   </threadedComment>
-  <threadedComment ref="J20" dT="2021-04-02T15:08:18.98" personId="{00000000-0000-0000-0000-000000000000}" id="{492F094F-8801-4499-80C3-4610B2EB4C3B}">
+  <threadedComment ref="J18" dT="2021-04-02T15:08:18.98" personId="{00000000-0000-0000-0000-000000000000}" id="{492F094F-8801-4499-80C3-4610B2EB4C3B}">
     <text>Boolean field -- indicates if sector has 2010 and 2090 impact esimates. Corresponds to impact year table below.</text>
   </threadedComment>
-  <threadedComment ref="D25" dT="2021-01-25T18:27:33.65" personId="{00000000-0000-0000-0000-000000000000}" id="{40274E0A-9A04-480D-A5E8-2C38F8B3CAD3}">
+  <threadedComment ref="D23" dT="2021-01-25T18:27:33.65" personId="{00000000-0000-0000-0000-000000000000}" id="{40274E0A-9A04-480D-A5E8-2C38F8B3CAD3}">
     <text>Empty values are replaced with "NA" in the R tool.</text>
   </threadedComment>
-  <threadedComment ref="E32" dT="2022-09-13T14:35:47.65" personId="{00000000-0000-0000-0000-000000000000}" id="{61FF9366-C253-4143-8900-DE7FDB924463}">
+  <threadedComment ref="E30" dT="2022-09-13T14:35:47.65" personId="{00000000-0000-0000-0000-000000000000}" id="{61FF9366-C253-4143-8900-DE7FDB924463}">
     <text>No spaces in this ID!</text>
   </threadedComment>
-  <threadedComment ref="F32" dT="2021-04-02T15:18:13.84" personId="{00000000-0000-0000-0000-000000000000}" id="{7C7D377F-2B53-48B7-807A-23CFCBC48B83}">
+  <threadedComment ref="F30" dT="2021-04-02T15:18:13.84" personId="{00000000-0000-0000-0000-000000000000}" id="{7C7D377F-2B53-48B7-807A-23CFCBC48B83}">
     <text>For sectors with multiple variants, one variant is considered the "primary" variant -- e.g., as used in when aggregating across sectors.</text>
   </threadedComment>
-  <threadedComment ref="G32" dT="2021-04-02T15:33:36.18" personId="{00000000-0000-0000-0000-000000000000}" id="{3962DDEC-520D-4477-AB4D-6A758B04F9CC}">
+  <threadedComment ref="G30" dT="2021-04-02T15:33:36.18" personId="{00000000-0000-0000-0000-000000000000}" id="{3962DDEC-520D-4477-AB4D-6A758B04F9CC}">
     <text>Numeric field -- indicates whether a sector should be included when aggregating over sectors. Sectors with a flag &gt;= 1 are generally included in aggregation. Flags &gt; 1 may have different treatments</text>
   </threadedComment>
-  <threadedComment ref="F46" dT="2021-04-02T15:36:58.50" personId="{00000000-0000-0000-0000-000000000000}" id="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
+  <threadedComment ref="F44" dT="2021-04-02T15:36:58.50" personId="{00000000-0000-0000-0000-000000000000}" id="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
     <text>This field tracks whether the input scalar is a time series of scalars, or a single input used to calculate a trajectory of the scalar in R. "Dynamic" scalars are a full series; "constant" are a single value from which a series is calculated in the R script.</text>
   </threadedComment>
-  <threadedComment ref="J62" dT="2021-02-11T17:01:11.40" personId="{00000000-0000-0000-0000-000000000000}" id="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
+  <threadedComment ref="J60" dT="2021-02-11T17:01:11.40" personId="{00000000-0000-0000-0000-000000000000}" id="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
     <text>Year when change and impacts are zero</text>
   </threadedComment>
-  <threadedComment ref="L62" dT="2021-02-15T18:58:52.31" personId="{00000000-0000-0000-0000-000000000000}" id="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
+  <threadedComment ref="L60" dT="2021-02-15T18:58:52.31" personId="{00000000-0000-0000-0000-000000000000}" id="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
     <text>Maximum value to extrapolate to, for models that go up to the maximum output value.</text>
   </threadedComment>
-  <threadedComment ref="D68" dT="2023-12-08T22:41:08.83" personId="{00000000-0000-0000-0000-000000000000}" id="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
+  <threadedComment ref="D66" dT="2023-12-08T22:41:08.83" personId="{00000000-0000-0000-0000-000000000000}" id="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
     <text>Max extrapolation temperature</text>
   </threadedComment>
-  <threadedComment ref="J80" dT="2021-03-30T17:10:38.36" personId="{00000000-0000-0000-0000-000000000000}" id="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
+  <threadedComment ref="J78" dT="2021-03-30T17:10:38.36" personId="{00000000-0000-0000-0000-000000000000}" id="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
     <text>Whether region is a dimension of the input</text>
   </threadedComment>
 </ThreadedComments>
@@ -7148,7 +7142,7 @@
   </sheetPr>
   <dimension ref="B9:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD34"/>
     </sheetView>
   </sheetViews>
@@ -7163,7 +7157,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7171,7 +7165,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="32.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -7179,13 +7173,13 @@
         <v>131</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="2:3" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="B12" s="48"/>
       <c r="C12" s="51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="2:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7285,7 +7279,7 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="B14" sqref="A14:XFD14"/>
@@ -7374,7 +7368,7 @@
       </c>
       <c r="G4" s="26" cm="1">
         <f t="array" aca="1" ref="G4" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H4" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7382,7 +7376,7 @@
       </c>
       <c r="I4" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J4" s="26" cm="1">
         <f t="array" aca="1" ref="J4" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7401,7 +7395,7 @@
         <v>10, 11, 12, 13, 14</v>
       </c>
       <c r="N4" s="41" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7410,7 +7404,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D5" s="22">
         <v>1</v>
@@ -7424,7 +7418,7 @@
       </c>
       <c r="G5" s="26" cm="1">
         <f t="array" aca="1" ref="G5" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H5" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7432,7 +7426,7 @@
       </c>
       <c r="I5" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J5" s="26" cm="1">
         <f t="array" aca="1" ref="J5" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7453,7 +7447,7 @@
         <v>8</v>
       </c>
       <c r="N5" s="41" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -7476,7 +7470,7 @@
       </c>
       <c r="G6" s="26" cm="1">
         <f t="array" aca="1" ref="G6" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H6" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7484,7 +7478,7 @@
       </c>
       <c r="I6" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J6" s="26" cm="1">
         <f t="array" aca="1" ref="J6" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7523,7 +7517,7 @@
       </c>
       <c r="G7" s="26" cm="1">
         <f t="array" aca="1" ref="G7" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H7" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7531,7 +7525,7 @@
       </c>
       <c r="I7" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J7" s="26" cm="1">
         <f t="array" aca="1" ref="J7" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7570,7 +7564,7 @@
       </c>
       <c r="G8" s="26" cm="1">
         <f t="array" aca="1" ref="G8" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H8" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7578,7 +7572,7 @@
       </c>
       <c r="I8" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8" s="26" cm="1">
         <f t="array" aca="1" ref="J8" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7617,7 +7611,7 @@
       </c>
       <c r="G9" s="26" cm="1">
         <f t="array" aca="1" ref="G9" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H9" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7625,7 +7619,7 @@
       </c>
       <c r="I9" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J9" s="26" cm="1">
         <f t="array" aca="1" ref="J9" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7664,7 +7658,7 @@
       </c>
       <c r="G10" s="26" cm="1">
         <f t="array" aca="1" ref="G10" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H10" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7672,7 +7666,7 @@
       </c>
       <c r="I10" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J10" s="26" cm="1">
         <f t="array" aca="1" ref="J10" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7711,7 +7705,7 @@
       </c>
       <c r="G11" s="26" cm="1">
         <f t="array" aca="1" ref="G11" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7719,7 +7713,7 @@
       </c>
       <c r="I11" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J11" s="26" cm="1">
         <f t="array" aca="1" ref="J11" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7761,7 +7755,7 @@
       </c>
       <c r="G12" s="26" cm="1">
         <f t="array" aca="1" ref="G12" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7769,7 +7763,7 @@
       </c>
       <c r="I12" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J12" s="26" cm="1">
         <f t="array" aca="1" ref="J12" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7794,7 +7788,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D13" s="22">
         <v>1</v>
@@ -7808,7 +7802,7 @@
       </c>
       <c r="G13" s="26" cm="1">
         <f t="array" aca="1" ref="G13" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H13" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7816,7 +7810,7 @@
       </c>
       <c r="I13" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J13" s="26" cm="1">
         <f t="array" aca="1" ref="J13" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7832,7 +7826,7 @@
       </c>
       <c r="M13" s="42"/>
       <c r="N13" s="41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -7841,13 +7835,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D14" s="22">
         <v>1</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" si="2"/>
@@ -7879,7 +7873,7 @@
       </c>
       <c r="M14" s="42"/>
       <c r="N14" s="41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -7888,7 +7882,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D15" s="22">
         <v>1</v>
@@ -7902,7 +7896,7 @@
       </c>
       <c r="G15" s="26" cm="1">
         <f t="array" aca="1" ref="G15" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H15" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7910,7 +7904,7 @@
       </c>
       <c r="I15" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J15" s="26" cm="1">
         <f t="array" aca="1" ref="J15" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7926,7 +7920,7 @@
       </c>
       <c r="M15" s="42"/>
       <c r="N15" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -7945,11 +7939,11 @@
   <sheetPr codeName="Sheet15">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U148"/>
+  <dimension ref="A1:U146"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A51" sqref="A51:XFD51"/>
+      <selection pane="topRight" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7997,7 +7991,7 @@
         <v>Sectors Table</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -8006,7 +8000,7 @@
         <v>Impact Year Estimates</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -8015,7 +8009,7 @@
         <v>Variants Table</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -8024,7 +8018,7 @@
         <v>Impact Types</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -8033,7 +8027,7 @@
         <v>Scalar Information</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -8042,13 +8036,13 @@
         <v>Economic Multipliers</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C8" s="43" t="e">
-        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( #REF! ), COLUMN( #REF! ), , , ) ), -2, , 1, 1 )</f>
-        <v>#REF!</v>
+      <c r="C8" s="43" t="str">
+        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_modelTypes[[#Headers],[row_id]] ), COLUMN( co_modelTypes[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
+        <v>Model Types</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>153</v>
@@ -8056,8 +8050,8 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C9" s="43" t="str">
-        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_modelTypes[[#Headers],[row_id]] ), COLUMN( co_modelTypes[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
-        <v>Model Types</v>
+        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_models[[#Headers],[row_id]] ), COLUMN( co_models[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
+        <v>GCM Models &amp; SLR Scenarios</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>154</v>
@@ -8065,281 +8059,291 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C10" s="43" t="str">
-        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_models[[#Headers],[row_id]] ), COLUMN( co_models[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
-        <v>GCM Models &amp; SLR Scenarios</v>
+        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_regions[[#Headers],[row_id]] ), COLUMN( co_regions[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
+        <v>Regions</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C11" s="43" t="str">
-        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_regions[[#Headers],[row_id]] ), COLUMN( co_regions[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
-        <v>Regions</v>
+        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_inputInfo[[#Headers],[row_id]] ), COLUMN( co_inputInfo[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
+        <v>Input Scenario Information</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C12" s="43" t="str">
-        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_inputInfo[[#Headers],[row_id]] ), COLUMN( co_inputInfo[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
-        <v>Input Scenario Information</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C13" s="43" t="str">
         <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_states[[#Headers],[row_id]] ), COLUMN( co_states[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
         <v>States</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C14" s="43" t="e">
-        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW(#REF! ), COLUMN(#REF! ), , , ) ), -3, , 1, 1 )</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="C16" s="47" t="s">
+      <c r="D12" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C14" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D14" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E14" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="F16" s="46" t="s">
+      <c r="F14" s="46" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15" t="s">
+    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-    </row>
-    <row r="20" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B20" s="16" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+    </row>
+    <row r="18" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B18" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E18" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F18" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G18" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="M18" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="H20" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="J20" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="L20" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="M20" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="N20" s="18" t="s">
+      <c r="N18" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="O20" s="18" t="s">
+      <c r="O18" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B21" s="57">
+    <row r="19" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B19" s="57">
         <f xml:space="preserve"> ROW( co_sectors[[#This Row],[row_id]] ) - ROW( co_sectors[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C19" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="E21" s="11">
+      <c r="D19" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="E19" s="11">
         <v>1</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="G21" s="66" t="str" cm="1">
-        <f t="array" aca="1" ref="G21" ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
+      <c r="G19" s="66" t="str" cm="1">
+        <f t="array" aca="1" ref="G19" ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_variants[[#Headers],[row_id]] ),  COLUMN( co_variants[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_variants[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_variants[variant_label], "" )
 )</f>
         <v>2011 Emissions, 2040 Emissions</v>
       </c>
-      <c r="H21" s="66" t="str">
+      <c r="H19" s="66" t="str">
         <f ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   OFFSET( INDIRECT( ADDRESS( ROW( INDEX( co_impactYears[sector_id], MATCH( co_sectors[[#This Row],[sector_id]], co_impactYears[sector_id], 0 ) ) ),  COLUMN( co_impactYears[[#Headers],[sector_id]] ), , , "controlTables" ) ), 0, 1, 1, 4 )
 )</f>
         <v>NA</v>
       </c>
-      <c r="I21" s="66" t="str" cm="1">
-        <f t="array" aca="1" ref="I21" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
+      <c r="I19" s="66" t="str" cm="1">
+        <f t="array" aca="1" ref="I19" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_impactTypes[[#Headers],[row_id]] ),  COLUMN( co_impactTypes[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_impactTypes[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_impactTypes[impactType_label], "" )
 )</f>
         <v>Ozone, PM2.5</v>
       </c>
-      <c r="J21" s="19">
+      <c r="J19" s="19">
         <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="68" t="b" cm="1">
-        <f t="array" ref="K21" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[physicalmeasure] = "N/A", 0, 1) ) &gt;= 1</f>
+      <c r="K19" s="68" t="b" cm="1">
+        <f t="array" ref="K19" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[physicalmeasure] = "N/A", 0, 1) ) &gt;= 1</f>
         <v>1</v>
       </c>
-      <c r="L21" s="68" t="b" cm="1">
-        <f t="array" ref="L21" xml:space="preserve"> OR( SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c0] &lt;&gt; 0, 1, 0) ) &gt;= 1,
+      <c r="L19" s="68" t="b" cm="1">
+        <f t="array" ref="L19" xml:space="preserve"> OR( SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c0] &lt;&gt; 0, 1, 0) ) &gt;= 1,
       SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c1] &lt;&gt; 0, 1, 0) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
-      <c r="M21" s="68" cm="1">
-        <f t="array" ref="M21" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
+      <c r="M19" s="68" cm="1">
+        <f t="array" ref="M19" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="N21" s="68" cm="1">
-        <f t="array" ref="N21" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
+      <c r="N19" s="68" cm="1">
+        <f t="array" ref="N19" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="O21" s="68" t="e" cm="1">
-        <f t="array" ref="O21" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+      <c r="O19" s="68" t="e" cm="1">
+        <f t="array" ref="O19" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15" t="s">
+    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="15"/>
-      <c r="T23" s="15"/>
-      <c r="U23" s="15"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B25" s="24" t="s">
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B23" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C23" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D23" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E23" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F25" s="26" t="s">
+      <c r="F23" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B26" s="4">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B24" s="4">
         <f xml:space="preserve"> ROW( co_impactYears[[#This Row],[row_id]] ) - ROW(co_impactYears[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D24" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="62" t="s">
+      <c r="E24" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F24" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15" t="s">
+    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="15"/>
+      <c r="O26" s="15"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
+      <c r="S26" s="15"/>
+      <c r="T26" s="15"/>
+      <c r="U26" s="15"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -8351,404 +8355,439 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B30" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
+    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B30" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
+      <c r="E30" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G30" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="41">
+        <v>2011</v>
+      </c>
+      <c r="F31" s="22">
+        <v>1</v>
+      </c>
+      <c r="G31" s="22">
+        <v>1</v>
+      </c>
+      <c r="H31" s="40" t="str">
+        <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
+   IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
+        <v>none</v>
+      </c>
+      <c r="I31" s="29" cm="1">
+        <f t="array" ref="I31" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
+        <v>1</v>
+      </c>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
     </row>
     <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="D32" s="37" t="s">
-        <v>201</v>
-      </c>
-      <c r="E32" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="F32" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="G32" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="H32" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
+      <c r="B32" s="4">
+        <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="41">
+        <v>2040</v>
+      </c>
+      <c r="F32" s="22">
+        <v>0</v>
+      </c>
+      <c r="G32" s="22">
+        <v>0</v>
+      </c>
+      <c r="H32" s="40" t="str">
+        <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
+   IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
+        <v>none</v>
+      </c>
+      <c r="I32" s="29" cm="1">
+        <f t="array" ref="I32" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
+        <v>1</v>
+      </c>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
     </row>
     <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="41">
-        <v>2011</v>
+        <v>18</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>101</v>
       </c>
       <c r="F33" s="22">
         <v>1</v>
       </c>
       <c r="G33" s="22">
-        <v>1</v>
-      </c>
-      <c r="H33" s="40" t="str">
+        <v>0</v>
+      </c>
+      <c r="H33" s="40" t="e">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
-        <v>none</v>
+        <v>#N/A</v>
       </c>
       <c r="I33" s="29" cm="1">
         <f t="array" ref="I33" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33"/>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
-        <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
-        <v>2</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" s="41">
-        <v>2040</v>
-      </c>
-      <c r="F34" s="22">
-        <v>0</v>
-      </c>
-      <c r="G34" s="22">
-        <v>0</v>
-      </c>
-      <c r="H34" s="40" t="str">
-        <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
-   IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
-        <v>none</v>
-      </c>
-      <c r="I34" s="29" cm="1">
-        <f t="array" ref="I34" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
-        <v>1</v>
-      </c>
-      <c r="J34"/>
-      <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
-    </row>
     <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B35" s="4">
-        <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
-        <v>3</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="F35" s="22">
-        <v>1</v>
-      </c>
-      <c r="G35" s="22">
-        <v>0</v>
-      </c>
-      <c r="H35" s="40" t="e">
-        <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
-   IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I35" s="29" cm="1">
-        <f t="array" ref="I35" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
-        <v>0</v>
-      </c>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-    </row>
-    <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="15" t="s">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="15"/>
-      <c r="Q37" s="15"/>
-      <c r="R37" s="15"/>
-      <c r="S37" s="15"/>
-      <c r="T37" s="15"/>
-      <c r="U37" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B37" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="J37" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="L37" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="M37" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="N37" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="O37" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="P37" s="26" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B38" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B39" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C39" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="G39" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="H39" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="I39" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="J39" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="K39" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="L39" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="M39" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="N39" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="O39" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="P39" s="26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B40" s="4">
+      <c r="B38" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D40" s="23" t="s">
+      <c r="D38" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="41" t="s">
+      <c r="E38" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="27" t="s">
+      <c r="F38" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="G38" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="H40" s="23" t="s">
+      <c r="H38" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I40" s="23" t="s">
+      <c r="I38" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="J38" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K40" s="23" t="s">
+      <c r="K38" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="L40" s="23" t="s">
+      <c r="L38" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="M40" s="22">
+      <c r="M38" s="22">
         <v>0</v>
       </c>
-      <c r="N40" s="22">
+      <c r="N38" s="22">
         <v>1</v>
       </c>
-      <c r="O40" s="22">
+      <c r="O38" s="22">
         <v>1</v>
       </c>
-      <c r="P40" s="28" t="str">
+      <c r="P38" s="28" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B41" s="4">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B39" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C39" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D39" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="E41" s="41" t="s">
+      <c r="E39" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="F41" s="27" t="s">
+      <c r="F39" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="G41" s="23" t="s">
+      <c r="G39" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="H41" s="23" t="s">
+      <c r="H39" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I41" s="23" t="s">
+      <c r="I39" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="J41" s="23" t="s">
+      <c r="J39" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K41" s="23" t="s">
+      <c r="K39" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="L41" s="23" t="s">
+      <c r="L39" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="M41" s="22">
+      <c r="M39" s="22">
         <v>0</v>
       </c>
-      <c r="N41" s="22">
+      <c r="N39" s="22">
         <v>1</v>
       </c>
-      <c r="O41" s="22">
+      <c r="O39" s="22">
         <v>1</v>
       </c>
-      <c r="P41" s="28" t="str">
+      <c r="P39" s="28" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
+    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="15"/>
+      <c r="L42" s="15"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="15"/>
+      <c r="R42" s="15"/>
+      <c r="S42" s="15"/>
+      <c r="T42" s="15"/>
+      <c r="U42" s="15"/>
+    </row>
     <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-    </row>
-    <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="24" t="s">
+      <c r="B44" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C44" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="D44" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="26" t="s">
+      <c r="E44" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="F46" s="26" t="s">
+      <c r="F44" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="G46" s="26" t="s">
+      <c r="G44" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="H46" s="26" t="s">
+      <c r="H44" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I46" s="26" t="s">
+      <c r="I44" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="J46" s="24" t="s">
+      <c r="J44" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5"/>
-    </row>
-    <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+    </row>
+    <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" s="6">
+        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="G45" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H45" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="J45" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B46" s="6">
+        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E46" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H46" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="J46" s="56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B47" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>41</v>
@@ -8757,7 +8796,7 @@
         <v>90</v>
       </c>
       <c r="E47" s="62" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F47" s="62" t="s">
         <v>60</v>
@@ -8774,14 +8813,11 @@
       <c r="J47" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="Q47"/>
-      <c r="R47"/>
-      <c r="S47"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B48" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>41</v>
@@ -8790,7 +8826,7 @@
         <v>90</v>
       </c>
       <c r="E48" s="62" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F48" s="62" t="s">
         <v>60</v>
@@ -8808,323 +8844,301 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B49" s="6">
-        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>3</v>
-      </c>
-      <c r="C49" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E49" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="F49" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="G49" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="H49" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="J49" s="56" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B50" s="6">
-        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>4</v>
-      </c>
-      <c r="C50" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D50" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E50" s="62" t="s">
-        <v>69</v>
-      </c>
-      <c r="F50" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="G50" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="H50" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="J50" s="56" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="15" t="s">
+    <row r="51" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="15"/>
-      <c r="T53" s="15"/>
-      <c r="U53" s="15"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B55" s="24" t="s">
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="15"/>
+      <c r="R51" s="15"/>
+      <c r="S51" s="15"/>
+      <c r="T51" s="15"/>
+      <c r="U51" s="15"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B53" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C55" s="24" t="s">
+      <c r="C53" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D55" s="24" t="s">
+      <c r="D53" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="E55" s="25" t="s">
+      <c r="E53" s="25" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B56" s="4">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B54" s="4">
         <f xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C54" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D56" s="38" t="s">
+      <c r="D54" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E56" s="39" t="s">
+      <c r="E54" s="39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="15" t="s">
+    <row r="58" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="14"/>
+      <c r="B58" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
-      <c r="P60" s="15"/>
-      <c r="Q60" s="15"/>
-      <c r="R60" s="15"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="15"/>
-      <c r="U60" s="15"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B62" s="31" t="s">
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
+      <c r="Q58" s="15"/>
+      <c r="R58" s="15"/>
+      <c r="S58" s="15"/>
+      <c r="T58" s="15"/>
+      <c r="U58" s="15"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B60" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C62" s="31" t="s">
+      <c r="C60" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D62" s="31" t="s">
+      <c r="D60" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="E62" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="F62" s="33" t="s">
+      <c r="E60" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="F60" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="G62" s="32" t="s">
+      <c r="G60" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="H62" s="32" t="s">
+      <c r="H60" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="I62" s="30" t="s">
+      <c r="I60" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="J62" s="30" t="s">
+      <c r="J60" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="K62" s="30" t="s">
+      <c r="K60" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="L62" s="30" t="s">
+      <c r="L60" s="30" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B63" s="4">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B61" s="4">
         <f xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C61" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D61" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E63" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="F63" s="35" t="s">
+      <c r="E61" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="F61" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="G63" s="34" t="s">
+      <c r="G61" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="H63" s="34" t="s">
+      <c r="H61" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="I63" s="36">
+      <c r="I61" s="36">
         <v>1</v>
       </c>
-      <c r="J63" s="36">
+      <c r="J61" s="36">
         <v>1995</v>
       </c>
-      <c r="K63" s="36">
+      <c r="K61" s="36">
         <v>6</v>
       </c>
-      <c r="L63" s="36">
+      <c r="L61" s="36">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
-      <c r="O66" s="15"/>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="15"/>
-      <c r="R66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="15"/>
-      <c r="U66" s="15"/>
+    <row r="64" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
+      <c r="S64" s="15"/>
+      <c r="T64" s="15"/>
+      <c r="U64" s="15"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B66" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D66" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="E66" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F66" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B67" s="4">
+        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C67" s="67" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
+        <v>CanESM2</v>
+      </c>
+      <c r="D67" s="38">
+        <v>6</v>
+      </c>
+      <c r="E67" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F67" s="65" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B68" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C68" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="D68" s="24" t="s">
-        <v>337</v>
-      </c>
-      <c r="E68" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F68" s="25" t="s">
-        <v>116</v>
+      <c r="B68" s="4">
+        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C68" s="67" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
+        <v>CCSM4</v>
+      </c>
+      <c r="D68" s="38">
+        <v>5</v>
+      </c>
+      <c r="E68" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F68" s="65" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B69" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C69" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>CanESM2</v>
+        <v>GISSE2R</v>
       </c>
       <c r="D69" s="38">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E69" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F69" s="65" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B70" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C70" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>CCSM4</v>
+        <v>HadGEM2ES</v>
       </c>
       <c r="D70" s="38">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E70" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F70" s="65" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B71" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C71" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>GISSE2R</v>
+        <v>MIROC5</v>
       </c>
       <c r="D71" s="38">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E71" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F71" s="65" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B72" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C72" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>HadGEM2ES</v>
+        <v>GFDLCM3</v>
       </c>
       <c r="D72" s="38">
         <v>6</v>
@@ -9133,1255 +9147,1216 @@
         <v>72</v>
       </c>
       <c r="F72" s="65" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B73" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C73" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>MIROC5</v>
+        <v>MRICGCM3</v>
       </c>
       <c r="D73" s="38">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E73" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F73" s="65" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B74" s="4">
-        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>6</v>
-      </c>
-      <c r="C74" s="67" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>GFDLCM3</v>
-      </c>
-      <c r="D74" s="38">
-        <v>6</v>
-      </c>
-      <c r="E74" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="F74" s="65" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B75" s="4">
-        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>7</v>
-      </c>
-      <c r="C75" s="67" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>MRICGCM3</v>
-      </c>
-      <c r="D75" s="38">
-        <v>3</v>
-      </c>
-      <c r="E75" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="F75" s="65" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
-      <c r="B78" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="14"/>
+      <c r="B76" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+      <c r="T76" s="15"/>
+      <c r="U76" s="15"/>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B78" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C78" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
-      <c r="H78" s="15"/>
-      <c r="I78" s="15"/>
-      <c r="J78" s="15"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="15"/>
-      <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="15"/>
-      <c r="P78" s="15"/>
-      <c r="Q78" s="15"/>
-      <c r="R78" s="15"/>
-      <c r="S78" s="15"/>
-      <c r="T78" s="15"/>
-      <c r="U78" s="15"/>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B80" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C80" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="D80" s="24" t="s">
+      <c r="D78" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="F78" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="E80" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="F80" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="G80" s="26" t="s">
+      <c r="G78" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="H78" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="H80" s="26" t="s">
+      <c r="I78" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="I80" s="26" t="s">
-        <v>174</v>
-      </c>
-      <c r="J80" s="26" t="s">
+      <c r="J78" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B81" s="4">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B79" s="4">
         <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C81" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D81" s="38" t="s">
+      <c r="C79" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D79" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="E81" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="F81" s="22" t="s">
+      <c r="E79" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="F79" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="G81" s="22">
+      <c r="G79" s="22">
         <v>0</v>
       </c>
-      <c r="H81" s="22"/>
-      <c r="I81" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="J81" s="22">
+      <c r="H79" s="22"/>
+      <c r="I79" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="J79" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B82" s="4">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B80" s="4">
         <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C80" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D82" s="38" t="s">
+      <c r="D80" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="E82" s="38" t="s">
-        <v>171</v>
-      </c>
-      <c r="F82" s="22" t="s">
+      <c r="E80" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="F80" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="G82" s="22">
+      <c r="G80" s="22">
         <v>0</v>
       </c>
-      <c r="H82" s="22"/>
-      <c r="I82" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="J82" s="22">
+      <c r="H80" s="22"/>
+      <c r="I80" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="J80" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
-      <c r="B85" s="15" t="s">
+    <row r="83" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="14"/>
+      <c r="B83" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C85" s="15"/>
-      <c r="D85" s="15"/>
-      <c r="E85" s="15"/>
-      <c r="F85" s="15"/>
-      <c r="G85" s="15"/>
-      <c r="H85" s="15"/>
-      <c r="I85" s="15"/>
-      <c r="J85" s="15"/>
-      <c r="K85" s="15"/>
-      <c r="L85" s="15"/>
-      <c r="M85" s="15"/>
-      <c r="N85" s="15"/>
-      <c r="O85" s="15"/>
-      <c r="P85" s="15"/>
-      <c r="Q85" s="15"/>
-      <c r="R85" s="15"/>
-      <c r="S85" s="15"/>
-      <c r="T85" s="15"/>
-      <c r="U85" s="15"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15"/>
+      <c r="P83" s="15"/>
+      <c r="Q83" s="15"/>
+      <c r="R83" s="15"/>
+      <c r="S83" s="15"/>
+      <c r="T83" s="15"/>
+      <c r="U83" s="15"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B85" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C85" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B86" s="4">
+        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C86" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="25" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
+        <v>Midwest</v>
+      </c>
+      <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B87" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C87" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D87" s="25" t="s">
-        <v>342</v>
+      <c r="B87" s="4">
+        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C87" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="25" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
+        <v>Northeast</v>
       </c>
       <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B88" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C88" s="38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D88" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Midwest</v>
+        <v>NorthernPlains</v>
       </c>
       <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B89" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C89" s="38" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D89" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Northeast</v>
+        <v>Northwest</v>
       </c>
       <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B90" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C90" s="38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D90" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>NorthernPlains</v>
+        <v>Southeast</v>
       </c>
       <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B91" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D91" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Northwest</v>
+        <v>SouthernPlains</v>
       </c>
       <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B92" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C92" s="38" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D92" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Southeast</v>
+        <v>Southwest</v>
       </c>
       <c r="E92" s="2"/>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B93" s="4">
-        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>6</v>
-      </c>
-      <c r="C93" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D93" s="25" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>SouthernPlains</v>
-      </c>
-      <c r="E93" s="2"/>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B94" s="4">
-        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>7</v>
-      </c>
-      <c r="C94" s="38" t="s">
+    <row r="95" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="14"/>
+      <c r="B95" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C95" s="15"/>
+      <c r="D95" s="15"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
+      <c r="L95" s="15"/>
+      <c r="M95" s="15"/>
+      <c r="N95" s="15"/>
+      <c r="O95" s="15"/>
+      <c r="P95" s="15"/>
+      <c r="Q95" s="15"/>
+      <c r="R95" s="15"/>
+      <c r="S95" s="15"/>
+      <c r="T95" s="15"/>
+      <c r="U95" s="15"/>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B97" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B98" s="2">
+        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
+        <v>1</v>
+      </c>
+      <c r="C98" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="D98" s="63" t="s">
+        <v>237</v>
+      </c>
+      <c r="E98" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B99" s="2">
+        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C99" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="D99" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="E99" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D94" s="25" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Southwest</v>
-      </c>
-      <c r="E94" s="2"/>
-    </row>
-    <row r="97" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
-      <c r="B97" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15"/>
-      <c r="E97" s="15"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="15"/>
-      <c r="H97" s="15"/>
-      <c r="I97" s="15"/>
-      <c r="J97" s="15"/>
-      <c r="K97" s="15"/>
-      <c r="L97" s="15"/>
-      <c r="M97" s="15"/>
-      <c r="N97" s="15"/>
-      <c r="O97" s="15"/>
-      <c r="P97" s="15"/>
-      <c r="Q97" s="15"/>
-      <c r="R97" s="15"/>
-      <c r="S97" s="15"/>
-      <c r="T97" s="15"/>
-      <c r="U97" s="15"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B99" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F99" s="64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B100" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C100" s="63" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D100" s="63" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E100" s="63" t="s">
         <v>10</v>
       </c>
       <c r="F100" s="64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B101" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C101" s="63" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D101" s="63" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="E101" s="63" t="s">
         <v>12</v>
       </c>
       <c r="F101" s="64">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B102" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C102" s="63" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D102" s="63" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E102" s="63" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F102" s="64">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B103" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C103" s="63" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D103" s="63" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="E103" s="63" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F103" s="64">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B104" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C104" s="63" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D104" s="63" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E104" s="63" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F104" s="64">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B105" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C105" s="63" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D105" s="63" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="E105" s="63" t="s">
         <v>7</v>
       </c>
       <c r="F105" s="64">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B106" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C106" s="63" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D106" s="63" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="E106" s="63" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F106" s="64">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B107" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C107" s="63" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D107" s="63" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="E107" s="63" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F107" s="64">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B108" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
+        <v>11</v>
+      </c>
+      <c r="C108" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="D108" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E108" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="C108" s="63" t="s">
-        <v>253</v>
-      </c>
-      <c r="D108" s="63" t="s">
-        <v>254</v>
-      </c>
-      <c r="E108" s="63" t="s">
-        <v>10</v>
-      </c>
       <c r="F108" s="64">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B109" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C109" s="63" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D109" s="63" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E109" s="63" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F109" s="64">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B110" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C110" s="63" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D110" s="63" t="s">
-        <v>20</v>
+        <v>260</v>
       </c>
       <c r="E110" s="63" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F110" s="64">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B111" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C111" s="63" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D111" s="63" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E111" s="63" t="s">
         <v>6</v>
       </c>
       <c r="F111" s="64">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B112" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C112" s="63" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D112" s="63" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="E112" s="63" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F112" s="64">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C113" s="63" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="D113" s="63" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="E113" s="63" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F113" s="64">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C114" s="63" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="D114" s="63" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="E114" s="63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F114" s="64">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B115" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C115" s="63" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D115" s="63" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="E115" s="63" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F115" s="64">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B116" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C116" s="63" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D116" s="63" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="E116" s="63" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F116" s="64">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B117" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C117" s="63" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="D117" s="63" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E117" s="63" t="s">
         <v>7</v>
       </c>
       <c r="F117" s="64">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B118" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C118" s="63" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="D118" s="63" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E118" s="63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F118" s="64">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B119" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C119" s="63" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="D119" s="63" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="E119" s="63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F119" s="64">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B120" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C120" s="63" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="D120" s="63" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="E120" s="63" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F120" s="64">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B121" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C121" s="63" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D121" s="63" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E121" s="63" t="s">
         <v>6</v>
       </c>
       <c r="F121" s="64">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B122" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C122" s="63" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="D122" s="63" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E122" s="63" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F122" s="64">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B123" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C123" s="63" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="D123" s="63" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E123" s="63" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F123" s="64">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B124" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C124" s="63" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D124" s="63" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E124" s="63" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F124" s="64">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B125" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C125" s="63" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D125" s="63" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E125" s="63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F125" s="64">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B126" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C126" s="63" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="D126" s="63" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="E126" s="63" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F126" s="64">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B127" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C127" s="63" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="D127" s="63" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="E127" s="63" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F127" s="64">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B128" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C128" s="63" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D128" s="63" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="E128" s="63" t="s">
         <v>7</v>
       </c>
       <c r="F128" s="64">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B129" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C129" s="63" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D129" s="63" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="E129" s="63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F129" s="64">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B130" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C130" s="63" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="D130" s="63" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="E130" s="63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F130" s="64">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B131" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C131" s="63" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D131" s="63" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="E131" s="63" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F131" s="64">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B132" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C132" s="63" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D132" s="63" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E132" s="63" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F132" s="64">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B133" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C133" s="63" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D133" s="63" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="E133" s="63" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F133" s="64">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B134" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C134" s="63" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D134" s="63" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E134" s="63" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F134" s="64">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B135" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C135" s="63" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D135" s="63" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E135" s="63" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F135" s="64">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B136" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C136" s="63" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D136" s="63" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E136" s="63" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F136" s="64">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B137" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C137" s="63" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D137" s="63" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="E137" s="63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F137" s="64">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B138" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C138" s="63" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="D138" s="63" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E138" s="63" t="s">
         <v>10</v>
       </c>
       <c r="F138" s="64">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B139" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C139" s="63" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D139" s="63" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E139" s="63" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F139" s="64">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B140" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C140" s="63" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D140" s="63" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E140" s="63" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F140" s="64">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B141" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C141" s="63" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D141" s="63" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E141" s="63" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F141" s="64">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B142" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C142" s="63" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D142" s="63" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E142" s="63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F142" s="64">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B143" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C143" s="63" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="D143" s="63" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="E143" s="63" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F143" s="64">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B144" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C144" s="63" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="D144" s="63" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="E144" s="63" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F144" s="64">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B145" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C145" s="63" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D145" s="63" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="E145" s="63" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F145" s="64">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B146" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C146" s="63" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="D146" s="63" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="E146" s="63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F146" s="64">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B147" s="2">
-        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>48</v>
-      </c>
-      <c r="C147" s="63" t="s">
-        <v>330</v>
-      </c>
-      <c r="D147" s="63" t="s">
-        <v>331</v>
-      </c>
-      <c r="E147" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="F147" s="64">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B148" s="2">
-        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>49</v>
-      </c>
-      <c r="C148" s="63" t="s">
-        <v>332</v>
-      </c>
-      <c r="D148" s="63" t="s">
-        <v>333</v>
-      </c>
-      <c r="E148" s="63" t="s">
-        <v>8</v>
-      </c>
-      <c r="F148" s="64">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="B21:F21">
+  <conditionalFormatting sqref="B19:F19">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula xml:space="preserve"> IF( $E21 = 1, 1, 0)</formula>
+      <formula xml:space="preserve"> IF( $E19 = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C8" location="loc_coConstants" display="loc_coConstants" xr:uid="{CFEFD72E-F9ED-4608-B7DD-AFDCEAF6F41D}"/>
-    <hyperlink ref="C10" location="loc_coModels" display="loc_coModels" xr:uid="{1AB1FA05-ED11-4F07-8B38-FA24CC6D4F4F}"/>
-    <hyperlink ref="C9" location="loc_coModelTypes" display="loc_coModelTypes" xr:uid="{DCB9BCCC-30A5-4252-A90A-CD0112FF06A8}"/>
+    <hyperlink ref="C9" location="loc_coModels" display="loc_coModels" xr:uid="{1AB1FA05-ED11-4F07-8B38-FA24CC6D4F4F}"/>
+    <hyperlink ref="C8" location="loc_coModelTypes" display="loc_coModelTypes" xr:uid="{DCB9BCCC-30A5-4252-A90A-CD0112FF06A8}"/>
     <hyperlink ref="C6" location="loc_coScalars" display="loc_coScalars" xr:uid="{9B32F273-E2BC-47BF-A60E-7A67D15D4D38}"/>
     <hyperlink ref="C7" location="loc_econMultipliers" display="loc_econMultipliers" xr:uid="{718FB73A-562F-40A4-9DCC-F7B32D89CA2B}"/>
     <hyperlink ref="C2" location="loc_coSectors" display="loc_coSectors" xr:uid="{0561FE55-51F9-468F-AA02-79E8761039B2}"/>
-    <hyperlink ref="C11" location="loc_coRegions" display="loc_coRegions" xr:uid="{A2DFA603-87D5-4136-9543-B92064985F7D}"/>
+    <hyperlink ref="C10" location="loc_coRegions" display="loc_coRegions" xr:uid="{A2DFA603-87D5-4136-9543-B92064985F7D}"/>
     <hyperlink ref="C3" location="loc_coImpactYears" display="loc_coImpactYears" xr:uid="{64F94EF8-131F-4A43-BC1A-C2AA36072515}"/>
     <hyperlink ref="C5" location="loc_coImpactTypes" display="loc_coImpactTypes" xr:uid="{114E9DA3-56F7-4D1E-B736-84EC6F366C11}"/>
     <hyperlink ref="C4" location="loc_coAdaptations" display="loc_coAdaptations" xr:uid="{7F53C6E9-E95F-4F38-8BCD-343D7DB6286E}"/>
-    <hyperlink ref="C12" location="loc_coInputScenarioInfo" display="loc_coInputScenarioInfo" xr:uid="{DA18E986-20B5-4E54-BA62-B58518D13EF3}"/>
-    <hyperlink ref="C13" location="loc_coStates" display="loc_coStates" xr:uid="{8BF3847D-2A5D-4A55-BC5A-0B347ED52535}"/>
+    <hyperlink ref="C11" location="loc_coInputScenarioInfo" display="loc_coInputScenarioInfo" xr:uid="{DA18E986-20B5-4E54-BA62-B58518D13EF3}"/>
+    <hyperlink ref="C12" location="loc_coStates" display="loc_coStates" xr:uid="{8BF3847D-2A5D-4A55-BC5A-0B347ED52535}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10422,7 +10397,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -10433,13 +10408,13 @@
         <v>22</v>
       </c>
       <c r="D3" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="53" t="s">
         <v>186</v>
       </c>
-      <c r="E3" s="53" t="s">
-        <v>187</v>
-      </c>
       <c r="F3" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="75" x14ac:dyDescent="0.25">
@@ -10457,7 +10432,7 @@
         <v>55</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -10475,12 +10450,12 @@
         <v>55</v>
       </c>
       <c r="F5" s="55" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -10491,10 +10466,10 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" t="s">
         <v>186</v>
-      </c>
-      <c r="E9" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -10634,10 +10609,10 @@
         <v>29</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -10649,10 +10624,10 @@
         <v>33</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>207</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -10664,10 +10639,10 @@
         <v>87</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -10676,13 +10651,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D6" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E6" s="41" t="s">
         <v>211</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10691,13 +10666,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -10709,10 +10684,10 @@
         <v>77</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10724,10 +10699,10 @@
         <v>78</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
@@ -10739,10 +10714,10 @@
         <v>79</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -10754,10 +10729,10 @@
         <v>32</v>
       </c>
       <c r="D11" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E11" s="41" t="s">
         <v>211</v>
-      </c>
-      <c r="E11" s="41" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -10769,10 +10744,10 @@
         <v>129</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10784,10 +10759,10 @@
         <v>93</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -10799,10 +10774,10 @@
         <v>130</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -10811,13 +10786,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D15" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="41" t="s">
         <v>211</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -10826,13 +10801,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="E16" s="41" t="s">
         <v>220</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10841,13 +10816,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17" s="41" t="s">
         <v>222</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -10856,13 +10831,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="E18" s="41" t="s">
         <v>224</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E18" s="41" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -10871,13 +10846,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D19" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E19" s="41" t="s">
         <v>211</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -10886,13 +10861,13 @@
         <v>17</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D20" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20" s="41" t="s">
         <v>211</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -10901,13 +10876,13 @@
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D21" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21" s="41" t="s">
         <v>211</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10916,13 +10891,13 @@
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="E22" s="41" t="s">
         <v>229</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Extremes module: initialized changes to functions to process and load the extremes data"
This reverts commit 43fb0ce1e12cbb7e2f9de39b189faa309ecb8571.
</commit_message>
<xml_diff>
--- a/inst/extdata/extremes/extremes_config.xlsx
+++ b/inst/extdata/extremes/extremes_config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7B04C17-C7AF-4455-BF2F-7B73916D67E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9002BBCD-34DF-4CC3-9303-AF285EF1BF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2865" yWindow="-25080" windowWidth="27555" windowHeight="18675" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7005" yWindow="-30225" windowWidth="27555" windowHeight="18675" tabRatio="764" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="48" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="loc_coImpactTypes">co_impactTypes[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coImpactYears">co_impactYears[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coInputScenarioInfo">co_inputInfo[[#Headers],[row_id]]</definedName>
-    <definedName name="loc_colorLegend">controlTables!$C$14</definedName>
+    <definedName name="loc_colorLegend">controlTables!$C$16</definedName>
     <definedName name="loc_coModels">co_models[[#Headers],[row_id]]</definedName>
     <definedName name="loc_coModelTypes">co_modelTypes[[#Headers],[row_id]]</definedName>
     <definedName name="loc_controlTOC">controlTables!$B$1</definedName>
@@ -35,8 +35,8 @@
     <definedName name="loc_coStates">co_impactYears[[#Headers],[row_id]]</definedName>
     <definedName name="loc_econMultipliers">co_econMultipliers[[#Headers],[row_id]]</definedName>
     <definedName name="num_gcms">MAX(co_models[row_id])</definedName>
-    <definedName name="SectorDropDown">controlTables!$D$19:$D$19</definedName>
-    <definedName name="SectorDropDown_1">controlTables!$D$19:$D$19</definedName>
+    <definedName name="SectorDropDown">controlTables!$D$21:$D$21</definedName>
+    <definedName name="SectorDropDown_1">controlTables!$D$21:$D$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -128,7 +128,7 @@
     <author>tc={A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}</author>
   </authors>
   <commentList>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{B1227AEC-55F2-4D4B-9D62-D8081C156293}">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{B1227AEC-55F2-4D4B-9D62-D8081C156293}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -136,7 +136,7 @@
     Boolean field -- indicates if sector is included in run of R script.</t>
       </text>
     </comment>
-    <comment ref="J18" authorId="1" shapeId="0" xr:uid="{492F094F-8801-4499-80C3-4610B2EB4C3B}">
+    <comment ref="J20" authorId="1" shapeId="0" xr:uid="{492F094F-8801-4499-80C3-4610B2EB4C3B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -144,7 +144,7 @@
     Boolean field -- indicates if sector has 2010 and 2090 impact esimates. Corresponds to impact year table below.</t>
       </text>
     </comment>
-    <comment ref="D23" authorId="2" shapeId="0" xr:uid="{40274E0A-9A04-480D-A5E8-2C38F8B3CAD3}">
+    <comment ref="D25" authorId="2" shapeId="0" xr:uid="{40274E0A-9A04-480D-A5E8-2C38F8B3CAD3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -152,7 +152,7 @@
     Empty values are replaced with "NA" in the R tool.</t>
       </text>
     </comment>
-    <comment ref="E30" authorId="3" shapeId="0" xr:uid="{61FF9366-C253-4143-8900-DE7FDB924463}">
+    <comment ref="E32" authorId="3" shapeId="0" xr:uid="{61FF9366-C253-4143-8900-DE7FDB924463}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -160,7 +160,7 @@
     No spaces in this ID!</t>
       </text>
     </comment>
-    <comment ref="F30" authorId="4" shapeId="0" xr:uid="{7C7D377F-2B53-48B7-807A-23CFCBC48B83}">
+    <comment ref="F32" authorId="4" shapeId="0" xr:uid="{7C7D377F-2B53-48B7-807A-23CFCBC48B83}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -168,7 +168,7 @@
     For sectors with multiple variants, one variant is considered the "primary" variant -- e.g., as used in when aggregating across sectors.</t>
       </text>
     </comment>
-    <comment ref="G30" authorId="5" shapeId="0" xr:uid="{3962DDEC-520D-4477-AB4D-6A758B04F9CC}">
+    <comment ref="G32" authorId="5" shapeId="0" xr:uid="{3962DDEC-520D-4477-AB4D-6A758B04F9CC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -176,7 +176,7 @@
     Numeric field -- indicates whether a sector should be included when aggregating over sectors. Sectors with a flag &gt;= 1 are generally included in aggregation. Flags &gt; 1 may have different treatments</t>
       </text>
     </comment>
-    <comment ref="F44" authorId="6" shapeId="0" xr:uid="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
+    <comment ref="F46" authorId="6" shapeId="0" xr:uid="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -184,7 +184,7 @@
     This field tracks whether the input scalar is a time series of scalars, or a single input used to calculate a trajectory of the scalar in R. "Dynamic" scalars are a full series; "constant" are a single value from which a series is calculated in the R script.</t>
       </text>
     </comment>
-    <comment ref="J60" authorId="7" shapeId="0" xr:uid="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
+    <comment ref="J62" authorId="7" shapeId="0" xr:uid="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -192,7 +192,7 @@
     Year when change and impacts are zero</t>
       </text>
     </comment>
-    <comment ref="L60" authorId="8" shapeId="0" xr:uid="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
+    <comment ref="L62" authorId="8" shapeId="0" xr:uid="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -200,7 +200,7 @@
     Maximum value to extrapolate to, for models that go up to the maximum output value.</t>
       </text>
     </comment>
-    <comment ref="D66" authorId="9" shapeId="0" xr:uid="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
+    <comment ref="D68" authorId="9" shapeId="0" xr:uid="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -208,7 +208,7 @@
     Max extrapolation temperature</t>
       </text>
     </comment>
-    <comment ref="J78" authorId="10" shapeId="0" xr:uid="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
+    <comment ref="J80" authorId="10" shapeId="0" xr:uid="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="346">
   <si>
     <t>CanESM2</t>
   </si>
@@ -702,6 +702,9 @@
   </si>
   <si>
     <t>Hard-coded value/included in model</t>
+  </si>
+  <si>
+    <t>Named constants</t>
   </si>
   <si>
     <t>Temperature and SLR-binning model types</t>
@@ -1296,6 +1299,9 @@
   </si>
   <si>
     <t>maxUnitValue</t>
+  </si>
+  <si>
+    <t>Info on SLR scalars past 2090</t>
   </si>
   <si>
     <t>Climate-Driven Changes in Air Quality</t>
@@ -6431,9 +6437,9 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C2AD6E-F129-4852-8BB5-5A249C234872}" name="co_variants" displayName="co_variants" ref="B30:I33" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B31:I33">
-    <sortCondition ref="C31:C33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{16C2AD6E-F129-4852-8BB5-5A249C234872}" name="co_variants" displayName="co_variants" ref="B32:I35" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B33:I35">
+    <sortCondition ref="C33:C35"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{1BCFA006-CF85-4F3A-AC79-60916A48ED39}" name="row_id" dataDxfId="53" totalsRowDxfId="52">
@@ -6457,7 +6463,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B53:E54" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8C208A9D-6726-48D1-84E7-1F3146AFFCB6}" name="co_econMultipliers" displayName="co_econMultipliers" ref="B55:E56" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{B5687CDE-96CA-4DF3-A45A-B2EDE1CC9A93}" name="row_id" dataDxfId="36">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6471,7 +6477,7 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B78:J80" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{90989828-E88F-4E7D-9FFC-173F0C723DE9}" name="co_inputInfo" displayName="co_inputInfo" ref="B80:J82" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66AD6D28-7A41-4AD2-93FD-110433F1C5A5}" name="row_id" dataDxfId="30">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6492,8 +6498,8 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B97:F146" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="B97:F146" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}" name="co_states" displayName="co_states" ref="B99:F148" totalsRowShown="0" headerRowDxfId="21">
+  <autoFilter ref="B99:F148" xr:uid="{260FF6F7-3417-4AB0-990E-0C31BC977851}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B802A69B-2E07-40A2-ADE9-DCABCB2E04A6}" name="row_id" dataDxfId="20">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6602,10 +6608,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4FB08D13-3C4C-4BB6-9ED3-E44A55D938B0}" name="co_sectors" displayName="co_sectors" ref="B18:O19" totalsRowShown="0" headerRowDxfId="153" dataDxfId="151" headerRowBorderDxfId="152" tableBorderDxfId="150" totalsRowBorderDxfId="149">
-  <autoFilter ref="B18:O19" xr:uid="{4FB08D13-3C4C-4BB6-9ED3-E44A55D938B0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B19:O19">
-    <sortCondition ref="D19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4FB08D13-3C4C-4BB6-9ED3-E44A55D938B0}" name="co_sectors" displayName="co_sectors" ref="B20:O21" totalsRowShown="0" headerRowDxfId="153" dataDxfId="151" headerRowBorderDxfId="152" tableBorderDxfId="150" totalsRowBorderDxfId="149">
+  <autoFilter ref="B20:O21" xr:uid="{4FB08D13-3C4C-4BB6-9ED3-E44A55D938B0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B21:O21">
+    <sortCondition ref="D21"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="14" xr3:uid="{60C3EA8F-72E0-495B-8B73-6D682443C60B}" name="row_id" dataDxfId="148" totalsRowDxfId="147">
@@ -6655,7 +6661,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{80839C52-E413-4982-A35C-46B477F75688}" name="co_modelTypes" displayName="co_modelTypes" ref="B60:L61" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{80839C52-E413-4982-A35C-46B477F75688}" name="co_modelTypes" displayName="co_modelTypes" ref="B62:L63" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{11DFD282-93A9-4795-9369-6627D14BB282}" name="row_id" dataDxfId="118">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6676,7 +6682,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBCED586-17E1-4B5C-A781-976D1E5A11BF}" name="co_regions" displayName="co_regions" ref="B85:D92" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{DBCED586-17E1-4B5C-A781-976D1E5A11BF}" name="co_regions" displayName="co_regions" ref="B87:D94" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{18599272-3810-42BA-A220-485AFB1D6807}" name="row_id" dataDxfId="105">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6691,7 +6697,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B66:F73" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CD29BCDB-B6F2-4FB9-B21C-6B30EFCFDCE7}" name="co_models" displayName="co_models" ref="B68:F75" totalsRowShown="0" headerRowDxfId="102" dataDxfId="101">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BF1485BD-F9FE-4F5B-9D9F-D9CB3D918F44}" name="row_id" dataDxfId="100">
       <calculatedColumnFormula xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</calculatedColumnFormula>
@@ -6708,10 +6714,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FBBCD2EA-5DCC-406C-B109-DA7E04AF91C0}" name="co_impactYears" displayName="co_impactYears" ref="B23:F24" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
-  <autoFilter ref="B23:F24" xr:uid="{965CD6B2-887D-46C8-9D98-6C6AECBC7B1A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B24:F24">
-    <sortCondition ref="C24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FBBCD2EA-5DCC-406C-B109-DA7E04AF91C0}" name="co_impactYears" displayName="co_impactYears" ref="B25:F26" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+  <autoFilter ref="B25:F26" xr:uid="{965CD6B2-887D-46C8-9D98-6C6AECBC7B1A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B26:F26">
+    <sortCondition ref="C26"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{CDF8B6C0-3166-4A5F-954A-6DD921A48F0D}" name="row_id" dataDxfId="93" totalsRowDxfId="92">
@@ -6727,11 +6733,11 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BAD307D6-4C07-4313-AAAB-5A0F25B0CD27}" name="co_impactTypes" displayName="co_impactTypes" ref="B37:P39" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
-  <autoFilter ref="B37:P39" xr:uid="{E446364F-959A-4BFF-80B5-CD65050C4865}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B38:P39">
-    <sortCondition ref="C38:C39"/>
-    <sortCondition ref="D38:D39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{BAD307D6-4C07-4313-AAAB-5A0F25B0CD27}" name="co_impactTypes" displayName="co_impactTypes" ref="B39:P41" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+  <autoFilter ref="B39:P41" xr:uid="{E446364F-959A-4BFF-80B5-CD65050C4865}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B40:P41">
+    <sortCondition ref="C40:C41"/>
+    <sortCondition ref="D40:D41"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{3C0C87EC-3301-4189-A438-330FBC0C23CE}" name="row_id" dataDxfId="81">
@@ -6759,11 +6765,11 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B44:J48" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
-  <autoFilter ref="B44:J48" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B45:J48">
-    <sortCondition ref="E45:E48"/>
-    <sortCondition ref="C45:C48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}" name="co_scalarInfo" displayName="co_scalarInfo" ref="B46:J50" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+  <autoFilter ref="B46:J50" xr:uid="{7F79E836-A486-4549-B875-6F873C0BCABB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B47:J50">
+    <sortCondition ref="E47:E50"/>
+    <sortCondition ref="C47:C50"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{B5AB138C-E49F-456B-8F7B-6A701BD94314}" name="row_id" dataDxfId="64">
@@ -7099,37 +7105,37 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E18" dT="2021-04-02T15:07:48.34" personId="{00000000-0000-0000-0000-000000000000}" id="{B1227AEC-55F2-4D4B-9D62-D8081C156293}">
+  <threadedComment ref="E20" dT="2021-04-02T15:07:48.34" personId="{00000000-0000-0000-0000-000000000000}" id="{B1227AEC-55F2-4D4B-9D62-D8081C156293}">
     <text>Boolean field -- indicates if sector is included in run of R script.</text>
   </threadedComment>
-  <threadedComment ref="J18" dT="2021-04-02T15:08:18.98" personId="{00000000-0000-0000-0000-000000000000}" id="{492F094F-8801-4499-80C3-4610B2EB4C3B}">
+  <threadedComment ref="J20" dT="2021-04-02T15:08:18.98" personId="{00000000-0000-0000-0000-000000000000}" id="{492F094F-8801-4499-80C3-4610B2EB4C3B}">
     <text>Boolean field -- indicates if sector has 2010 and 2090 impact esimates. Corresponds to impact year table below.</text>
   </threadedComment>
-  <threadedComment ref="D23" dT="2021-01-25T18:27:33.65" personId="{00000000-0000-0000-0000-000000000000}" id="{40274E0A-9A04-480D-A5E8-2C38F8B3CAD3}">
+  <threadedComment ref="D25" dT="2021-01-25T18:27:33.65" personId="{00000000-0000-0000-0000-000000000000}" id="{40274E0A-9A04-480D-A5E8-2C38F8B3CAD3}">
     <text>Empty values are replaced with "NA" in the R tool.</text>
   </threadedComment>
-  <threadedComment ref="E30" dT="2022-09-13T14:35:47.65" personId="{00000000-0000-0000-0000-000000000000}" id="{61FF9366-C253-4143-8900-DE7FDB924463}">
+  <threadedComment ref="E32" dT="2022-09-13T14:35:47.65" personId="{00000000-0000-0000-0000-000000000000}" id="{61FF9366-C253-4143-8900-DE7FDB924463}">
     <text>No spaces in this ID!</text>
   </threadedComment>
-  <threadedComment ref="F30" dT="2021-04-02T15:18:13.84" personId="{00000000-0000-0000-0000-000000000000}" id="{7C7D377F-2B53-48B7-807A-23CFCBC48B83}">
+  <threadedComment ref="F32" dT="2021-04-02T15:18:13.84" personId="{00000000-0000-0000-0000-000000000000}" id="{7C7D377F-2B53-48B7-807A-23CFCBC48B83}">
     <text>For sectors with multiple variants, one variant is considered the "primary" variant -- e.g., as used in when aggregating across sectors.</text>
   </threadedComment>
-  <threadedComment ref="G30" dT="2021-04-02T15:33:36.18" personId="{00000000-0000-0000-0000-000000000000}" id="{3962DDEC-520D-4477-AB4D-6A758B04F9CC}">
+  <threadedComment ref="G32" dT="2021-04-02T15:33:36.18" personId="{00000000-0000-0000-0000-000000000000}" id="{3962DDEC-520D-4477-AB4D-6A758B04F9CC}">
     <text>Numeric field -- indicates whether a sector should be included when aggregating over sectors. Sectors with a flag &gt;= 1 are generally included in aggregation. Flags &gt; 1 may have different treatments</text>
   </threadedComment>
-  <threadedComment ref="F44" dT="2021-04-02T15:36:58.50" personId="{00000000-0000-0000-0000-000000000000}" id="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
+  <threadedComment ref="F46" dT="2021-04-02T15:36:58.50" personId="{00000000-0000-0000-0000-000000000000}" id="{EF83C059-A623-47AC-AFC4-40246F6AF9B2}">
     <text>This field tracks whether the input scalar is a time series of scalars, or a single input used to calculate a trajectory of the scalar in R. "Dynamic" scalars are a full series; "constant" are a single value from which a series is calculated in the R script.</text>
   </threadedComment>
-  <threadedComment ref="J60" dT="2021-02-11T17:01:11.40" personId="{00000000-0000-0000-0000-000000000000}" id="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
+  <threadedComment ref="J62" dT="2021-02-11T17:01:11.40" personId="{00000000-0000-0000-0000-000000000000}" id="{74E8C379-DF77-4FAE-8C13-4D0000C68271}">
     <text>Year when change and impacts are zero</text>
   </threadedComment>
-  <threadedComment ref="L60" dT="2021-02-15T18:58:52.31" personId="{00000000-0000-0000-0000-000000000000}" id="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
+  <threadedComment ref="L62" dT="2021-02-15T18:58:52.31" personId="{00000000-0000-0000-0000-000000000000}" id="{984021BA-DD3F-4758-AAFF-698CBFB1E97F}">
     <text>Maximum value to extrapolate to, for models that go up to the maximum output value.</text>
   </threadedComment>
-  <threadedComment ref="D66" dT="2023-12-08T22:41:08.83" personId="{00000000-0000-0000-0000-000000000000}" id="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
+  <threadedComment ref="D68" dT="2023-12-08T22:41:08.83" personId="{00000000-0000-0000-0000-000000000000}" id="{A0D64BDD-1681-4C8F-9929-C1898D0603B0}">
     <text>Max extrapolation temperature</text>
   </threadedComment>
-  <threadedComment ref="J78" dT="2021-03-30T17:10:38.36" personId="{00000000-0000-0000-0000-000000000000}" id="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
+  <threadedComment ref="J80" dT="2021-03-30T17:10:38.36" personId="{00000000-0000-0000-0000-000000000000}" id="{A5816E78-F7FA-40E3-ACC3-4CDB677E4DA9}">
     <text>Whether region is a dimension of the input</text>
   </threadedComment>
 </ThreadedComments>
@@ -7142,7 +7148,7 @@
   </sheetPr>
   <dimension ref="B9:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD34"/>
     </sheetView>
   </sheetViews>
@@ -7157,7 +7163,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7165,7 +7171,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="32.25" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
@@ -7173,13 +7179,13 @@
         <v>131</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="2:3" hidden="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="B12" s="48"/>
       <c r="C12" s="51" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="2:3" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -7279,7 +7285,7 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B3" workbookViewId="0">
       <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="B14" sqref="A14:XFD14"/>
@@ -7368,7 +7374,7 @@
       </c>
       <c r="G4" s="26" cm="1">
         <f t="array" aca="1" ref="G4" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H4" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7376,7 +7382,7 @@
       </c>
       <c r="I4" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J4" s="26" cm="1">
         <f t="array" aca="1" ref="J4" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7395,7 +7401,7 @@
         <v>10, 11, 12, 13, 14</v>
       </c>
       <c r="N4" s="41" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7404,7 +7410,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D5" s="22">
         <v>1</v>
@@ -7418,7 +7424,7 @@
       </c>
       <c r="G5" s="26" cm="1">
         <f t="array" aca="1" ref="G5" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H5" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7426,7 +7432,7 @@
       </c>
       <c r="I5" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J5" s="26" cm="1">
         <f t="array" aca="1" ref="J5" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7447,7 +7453,7 @@
         <v>8</v>
       </c>
       <c r="N5" s="41" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -7470,7 +7476,7 @@
       </c>
       <c r="G6" s="26" cm="1">
         <f t="array" aca="1" ref="G6" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H6" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7478,7 +7484,7 @@
       </c>
       <c r="I6" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J6" s="26" cm="1">
         <f t="array" aca="1" ref="J6" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7517,7 +7523,7 @@
       </c>
       <c r="G7" s="26" cm="1">
         <f t="array" aca="1" ref="G7" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H7" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7525,7 +7531,7 @@
       </c>
       <c r="I7" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J7" s="26" cm="1">
         <f t="array" aca="1" ref="J7" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7564,7 +7570,7 @@
       </c>
       <c r="G8" s="26" cm="1">
         <f t="array" aca="1" ref="G8" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H8" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7572,7 +7578,7 @@
       </c>
       <c r="I8" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J8" s="26" cm="1">
         <f t="array" aca="1" ref="J8" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7611,7 +7617,7 @@
       </c>
       <c r="G9" s="26" cm="1">
         <f t="array" aca="1" ref="G9" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H9" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7619,7 +7625,7 @@
       </c>
       <c r="I9" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J9" s="26" cm="1">
         <f t="array" aca="1" ref="J9" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7658,7 +7664,7 @@
       </c>
       <c r="G10" s="26" cm="1">
         <f t="array" aca="1" ref="G10" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H10" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7666,7 +7672,7 @@
       </c>
       <c r="I10" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J10" s="26" cm="1">
         <f t="array" aca="1" ref="J10" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7705,7 +7711,7 @@
       </c>
       <c r="G11" s="26" cm="1">
         <f t="array" aca="1" ref="G11" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H11" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7713,7 +7719,7 @@
       </c>
       <c r="I11" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J11" s="26" cm="1">
         <f t="array" aca="1" ref="J11" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7755,7 +7761,7 @@
       </c>
       <c r="G12" s="26" cm="1">
         <f t="array" aca="1" ref="G12" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H12" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7763,7 +7769,7 @@
       </c>
       <c r="I12" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J12" s="26" cm="1">
         <f t="array" aca="1" ref="J12" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7788,7 +7794,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D13" s="22">
         <v>1</v>
@@ -7802,7 +7808,7 @@
       </c>
       <c r="G13" s="26" cm="1">
         <f t="array" aca="1" ref="G13" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H13" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7810,7 +7816,7 @@
       </c>
       <c r="I13" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J13" s="26" cm="1">
         <f t="array" aca="1" ref="J13" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7826,7 +7832,7 @@
       </c>
       <c r="M13" s="42"/>
       <c r="N13" s="41" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -7835,13 +7841,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D14" s="22">
         <v>1</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F14" s="22" t="str">
         <f t="shared" si="2"/>
@@ -7873,7 +7879,7 @@
       </c>
       <c r="M14" s="42"/>
       <c r="N14" s="41" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -7882,7 +7888,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D15" s="22">
         <v>1</v>
@@ -7896,7 +7902,7 @@
       </c>
       <c r="G15" s="26" cm="1">
         <f t="array" aca="1" ref="G15" ca="1" xml:space="preserve"> INDEX( ROW( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[[#Headers],[", doc_tablesList[[#This Row],[ID_columnName]], "]]" ) ) ), 1 )</f>
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H15" s="26">
         <f ca="1" xml:space="preserve"> MAX( INDIRECT( _xlfn.TEXTJOIN( "", , doc_tablesList[[#This Row],[Table Name]], "[", doc_tablesList[[#This Row],[ID_columnName]], "]" ) ) )</f>
@@ -7904,7 +7910,7 @@
       </c>
       <c r="I15" s="26">
         <f ca="1" xml:space="preserve"> doc_tablesList[[#This Row],[Number of Data Rows]] + doc_tablesList[[#This Row],[Header Row]]</f>
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J15" s="26" cm="1">
         <f t="array" aca="1" ref="J15" ca="1" xml:space="preserve"> INDEX( COLUMN( INDIRECT( doc_tablesList[[#This Row],[Table Name]] &amp; "[" &amp; doc_tablesList[[#This Row],[ID_columnName]] &amp; "]" ) ), 1 )</f>
@@ -7920,7 +7926,7 @@
       </c>
       <c r="M15" s="42"/>
       <c r="N15" s="41" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -7939,11 +7945,11 @@
   <sheetPr codeName="Sheet15">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U146"/>
+  <dimension ref="A1:U148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C60" sqref="C60"/>
+      <selection pane="topRight" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7991,7 +7997,7 @@
         <v>Sectors Table</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -8000,7 +8006,7 @@
         <v>Impact Year Estimates</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -8009,7 +8015,7 @@
         <v>Variants Table</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -8018,7 +8024,7 @@
         <v>Impact Types</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -8027,7 +8033,7 @@
         <v>Scalar Information</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -8036,314 +8042,304 @@
         <v>Economic Multipliers</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C8" s="43" t="str">
+      <c r="C8" s="43" t="e">
+        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( #REF! ), COLUMN( #REF! ), , , ) ), -2, , 1, 1 )</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C9" s="43" t="str">
         <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_modelTypes[[#Headers],[row_id]] ), COLUMN( co_modelTypes[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
         <v>Model Types</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C9" s="43" t="str">
+      <c r="D9" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C10" s="43" t="str">
         <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_models[[#Headers],[row_id]] ), COLUMN( co_models[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
         <v>GCM Models &amp; SLR Scenarios</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C10" s="43" t="str">
+      <c r="D10" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C11" s="43" t="str">
         <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_regions[[#Headers],[row_id]] ), COLUMN( co_regions[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
         <v>Regions</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C11" s="43" t="str">
+      <c r="D11" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C12" s="43" t="str">
         <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_inputInfo[[#Headers],[row_id]] ), COLUMN( co_inputInfo[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
         <v>Input Scenario Information</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C12" s="43" t="str">
+      <c r="D12" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C13" s="43" t="str">
         <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW( co_states[[#Headers],[row_id]] ), COLUMN( co_states[[#Headers],[row_id]] ), , , ) ), -2, , 1, 1 )</f>
         <v>States</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="C14" s="47" t="s">
+      <c r="D13" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C14" s="43" t="e">
+        <f ca="1" xml:space="preserve"> OFFSET( INDIRECT( ADDRESS( ROW(#REF! ), COLUMN(#REF! ), , , ) ), -3, , 1, 1 )</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="C16" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D16" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E16" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="F14" s="46" t="s">
+      <c r="F16" s="46" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15" t="s">
+    <row r="18" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-    </row>
-    <row r="18" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B18" s="16" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+    </row>
+    <row r="20" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B20" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D20" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E20" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F20" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="G18" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="H18" s="18" t="s">
+      <c r="G20" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="H20" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="I20" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>342</v>
-      </c>
-      <c r="L18" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="M18" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="N18" s="18" t="s">
+      <c r="J20" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="M20" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="N20" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="O18" s="18" t="s">
+      <c r="O20" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B19" s="57">
+    <row r="21" spans="1:21" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B21" s="57">
         <f xml:space="preserve"> ROW( co_sectors[[#This Row],[row_id]] ) - ROW( co_sectors[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="C21" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="E19" s="11">
+      <c r="D21" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="E21" s="11">
         <v>1</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="66" t="str" cm="1">
-        <f t="array" aca="1" ref="G19" ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
+      <c r="G21" s="66" t="str" cm="1">
+        <f t="array" aca="1" ref="G21" ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_variants[[#Headers],[row_id]] ),  COLUMN( co_variants[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_variants[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_variants[variant_label], "" )
 )</f>
         <v>2011 Emissions, 2040 Emissions</v>
       </c>
-      <c r="H19" s="66" t="str">
+      <c r="H21" s="66" t="str">
         <f ca="1" xml:space="preserve"> _xlfn.TEXTJOIN( ", ", 1,
   OFFSET( INDIRECT( ADDRESS( ROW( INDEX( co_impactYears[sector_id], MATCH( co_sectors[[#This Row],[sector_id]], co_impactYears[sector_id], 0 ) ) ),  COLUMN( co_impactYears[[#Headers],[sector_id]] ), , , "controlTables" ) ), 0, 1, 1, 4 )
 )</f>
         <v>NA</v>
       </c>
-      <c r="I19" s="66" t="str" cm="1">
-        <f t="array" aca="1" ref="I19" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
+      <c r="I21" s="66" t="str" cm="1">
+        <f t="array" aca="1" ref="I21" ca="1" xml:space="preserve">  _xlfn.TEXTJOIN( ", ", 1,
   IF( OFFSET( INDIRECT( ADDRESS( ROW( co_impactTypes[[#Headers],[row_id]] ),  COLUMN( co_impactTypes[[#Headers],[sector_id]] ), , , "controlTables" ) ), 1, 0, MAX( co_impactTypes[row_id] ), 1 ) = co_sectors[[#This Row],[sector_id]], co_impactTypes[impactType_label], "" )
 )</f>
         <v>Ozone, PM2.5</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J21" s="19">
         <f ca="1" xml:space="preserve"> IF( co_sectors[[#This Row],[impactYears]] = "NA", 0, 1)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="68" t="b" cm="1">
-        <f t="array" ref="K19" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[physicalmeasure] = "N/A", 0, 1) ) &gt;= 1</f>
+      <c r="K21" s="68" t="b" cm="1">
+        <f t="array" ref="K21" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[physicalmeasure] = "N/A", 0, 1) ) &gt;= 1</f>
         <v>1</v>
       </c>
-      <c r="L19" s="68" t="b" cm="1">
-        <f t="array" ref="L19" xml:space="preserve"> OR( SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c0] &lt;&gt; 0, 1, 0) ) &gt;= 1,
+      <c r="L21" s="68" t="b" cm="1">
+        <f t="array" ref="L21" xml:space="preserve"> OR( SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c0] &lt;&gt; 0, 1, 0) ) &gt;= 1,
       SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ), --IF( co_impactTypes[c1] &lt;&gt; 0, 1, 0) ) &gt;= 1 )</f>
         <v>1</v>
       </c>
-      <c r="M19" s="68" cm="1">
-        <f t="array" ref="M19" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
+      <c r="M21" s="68" cm="1">
+        <f t="array" ref="M21" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_variants[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="N19" s="68" cm="1">
-        <f t="array" ref="N19" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
+      <c r="N21" s="68" cm="1">
+        <f t="array" ref="N21" xml:space="preserve"> SUMPRODUCT( --( co_sectors[[#This Row],[sector_id]] = co_impactTypes[sector_id] ) )</f>
         <v>2</v>
       </c>
-      <c r="O19" s="68" t="e" cm="1">
-        <f t="array" ref="O19" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
+      <c r="O21" s="68" t="e" cm="1">
+        <f t="array" ref="O21" xml:space="preserve"> IF( INDEX( co_impactYears[NA], MATCH( 1, --( co_sectors[[#This Row],[sector_id]] = co_impactYears[sector_id] ), 0 ) ) = "NA", 1, 2 )</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="15" t="s">
+    <row r="23" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B23" s="24" t="s">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B25" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C25" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D25" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E25" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F25" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="4">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B26" s="4">
         <f xml:space="preserve"> ROW( co_impactYears[[#This Row],[row_id]] ) - ROW(co_impactYears[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D26" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="62" t="s">
+      <c r="E26" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F26" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="15"/>
-      <c r="I26" s="15"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="15"/>
-      <c r="S26" s="15"/>
-      <c r="T26" s="15"/>
-      <c r="U26" s="15"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
+    <row r="28" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B28" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
+      <c r="S28" s="15"/>
+      <c r="T28" s="15"/>
+      <c r="U28" s="15"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -8355,440 +8351,405 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
-    <row r="30" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B30" s="37" t="s">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B32" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C32" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="37" t="s">
-        <v>200</v>
-      </c>
-      <c r="E30" s="37" t="s">
+      <c r="D32" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="F30" s="26" t="s">
+      <c r="E32" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="F32" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G32" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="H32" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I30" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-    </row>
-    <row r="31" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B31" s="4">
+      <c r="I32" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
         <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="E31" s="41">
+      <c r="E33" s="41">
         <v>2011</v>
       </c>
-      <c r="F31" s="22">
+      <c r="F33" s="22">
         <v>1</v>
       </c>
-      <c r="G31" s="22">
+      <c r="G33" s="22">
         <v>1</v>
       </c>
-      <c r="H31" s="40" t="str">
+      <c r="H33" s="40" t="str">
         <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
    IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
         <v>none</v>
       </c>
-      <c r="I31" s="29" cm="1">
-        <f t="array" ref="I31" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
-        <v>1</v>
-      </c>
-      <c r="J31"/>
-      <c r="K31"/>
-      <c r="L31"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B32" s="4">
-        <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
-        <v>2</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="41">
-        <v>2040</v>
-      </c>
-      <c r="F32" s="22">
-        <v>0</v>
-      </c>
-      <c r="G32" s="22">
-        <v>0</v>
-      </c>
-      <c r="H32" s="40" t="str">
-        <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
-   IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
-        <v>none</v>
-      </c>
-      <c r="I32" s="29" cm="1">
-        <f t="array" ref="I32" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
-        <v>1</v>
-      </c>
-      <c r="J32"/>
-      <c r="K32"/>
-      <c r="L32"/>
-      <c r="M32"/>
-    </row>
-    <row r="33" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B33" s="4">
-        <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
-        <v>3</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="F33" s="22">
-        <v>1</v>
-      </c>
-      <c r="G33" s="22">
-        <v>0</v>
-      </c>
-      <c r="H33" s="40" t="e">
-        <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
-   IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
-        <v>#N/A</v>
-      </c>
       <c r="I33" s="29" cm="1">
         <f t="array" ref="I33" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33"/>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33"/>
     </row>
+    <row r="34" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
+        <v>2</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="41">
+        <v>2040</v>
+      </c>
+      <c r="F34" s="22">
+        <v>0</v>
+      </c>
+      <c r="G34" s="22">
+        <v>0</v>
+      </c>
+      <c r="H34" s="40" t="str">
+        <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
+   IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
+        <v>none</v>
+      </c>
+      <c r="I34" s="29" cm="1">
+        <f t="array" ref="I34" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
+        <v>1</v>
+      </c>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+    </row>
     <row r="35" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="4">
+        <f xml:space="preserve"> ROW( co_variants[[#This Row],[row_id]] ) - ROW( co_variants[[#Headers],[row_id]] )</f>
+        <v>3</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="22">
+        <v>1</v>
+      </c>
+      <c r="G35" s="22">
+        <v>0</v>
+      </c>
+      <c r="H35" s="40" t="e">
+        <f xml:space="preserve"> INDEX( co_impactTypes[damageAdjName], MATCH( co_variants[[#This Row],[sector_id]], co_impactTypes[sector_id], 0 ) ) &amp;
+   IF( OR(co_variants[[#This Row],[sector_id]] = "Roads", co_variants[[#This Row],[sector_id]] = "ForestryLoss"),"_" &amp; co_variants[[#This Row],[variant_id]], "" )</f>
+        <v>#N/A</v>
+      </c>
+      <c r="I35" s="29" cm="1">
+        <f t="array" ref="I35" xml:space="preserve"> --( SUMPRODUCT( --( co_impactTypes[sector_id] = co_variants[[#This Row],[sector_id]] ) ) &gt;= 1 )</f>
+        <v>0</v>
+      </c>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+    </row>
+    <row r="37" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B36" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B37" s="24" t="s">
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B39" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C39" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D39" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E39" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F39" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="G39" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="H37" s="24" t="s">
+      <c r="H39" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="I37" s="24" t="s">
+      <c r="I39" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="J37" s="24" t="s">
+      <c r="J39" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="K37" s="24" t="s">
+      <c r="K39" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="L37" s="24" t="s">
+      <c r="L39" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="M37" s="26" t="s">
+      <c r="M39" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="N37" s="26" t="s">
+      <c r="N39" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="O37" s="26" t="s">
+      <c r="O39" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="P37" s="26" t="s">
+      <c r="P39" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B38" s="4">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B40" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C40" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D40" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="41" t="s">
+      <c r="E40" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="27" t="s">
+      <c r="F40" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="23" t="s">
+      <c r="G40" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="H38" s="23" t="s">
+      <c r="H40" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I38" s="23" t="s">
+      <c r="I40" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="J38" s="23" t="s">
+      <c r="J40" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K38" s="23" t="s">
+      <c r="K40" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="L38" s="23" t="s">
+      <c r="L40" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="M38" s="22">
+      <c r="M40" s="22">
         <v>0</v>
       </c>
-      <c r="N38" s="22">
+      <c r="N40" s="22">
         <v>1</v>
       </c>
-      <c r="O38" s="22">
+      <c r="O40" s="22">
         <v>1</v>
       </c>
-      <c r="P38" s="28" t="str">
+      <c r="P40" s="28" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B39" s="4">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B41" s="4">
         <f xml:space="preserve"> ROW( co_impactTypes[[#This Row],[row_id]] ) - ROW(co_impactTypes[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C41" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D41" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="41" t="s">
+      <c r="E41" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F41" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="G39" s="23" t="s">
+      <c r="G41" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="H39" s="23" t="s">
+      <c r="H41" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I39" s="23" t="s">
+      <c r="I41" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="J39" s="23" t="s">
+      <c r="J41" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K39" s="23" t="s">
+      <c r="K41" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="L39" s="23" t="s">
+      <c r="L41" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="M39" s="22">
+      <c r="M41" s="22">
         <v>0</v>
       </c>
-      <c r="N39" s="22">
+      <c r="N41" s="22">
         <v>1</v>
       </c>
-      <c r="O39" s="22">
+      <c r="O41" s="22">
         <v>1</v>
       </c>
-      <c r="P39" s="28" t="str">
+      <c r="P41" s="28" t="str">
         <f xml:space="preserve"> IF(co_impactTypes[[#This Row],[econMultiplierName]]="None", "N/A", 2010)</f>
         <v>N/A</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
-      <c r="P42" s="15"/>
-      <c r="Q42" s="15"/>
-      <c r="R42" s="15"/>
-      <c r="S42" s="15"/>
-      <c r="T42" s="15"/>
-      <c r="U42" s="15"/>
-    </row>
     <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="A44" s="14"/>
+      <c r="B44" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
+      <c r="U44" s="15"/>
+    </row>
+    <row r="46" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C46" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D44" s="24" t="s">
+      <c r="D46" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="26" t="s">
+      <c r="E46" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="F44" s="26" t="s">
+      <c r="F46" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="G44" s="26" t="s">
+      <c r="G46" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="H44" s="26" t="s">
+      <c r="H46" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="I44" s="26" t="s">
+      <c r="I46" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="J44" s="24" t="s">
+      <c r="J46" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-    </row>
-    <row r="45" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="B45" s="6">
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+    </row>
+    <row r="47" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C45" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="F45" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="G45" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="H45" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="I45" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="J45" s="56" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q45"/>
-      <c r="R45"/>
-      <c r="S45"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B46" s="6">
-        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>2</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="E46" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="F46" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="G46" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="H46" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="I46" s="42" t="s">
-        <v>89</v>
-      </c>
-      <c r="J46" s="56" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B47" s="6">
-        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>3</v>
-      </c>
       <c r="C47" s="27" t="s">
         <v>41</v>
       </c>
@@ -8796,7 +8757,7 @@
         <v>90</v>
       </c>
       <c r="E47" s="62" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F47" s="62" t="s">
         <v>60</v>
@@ -8813,11 +8774,14 @@
       <c r="J47" s="56" t="s">
         <v>91</v>
       </c>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B48" s="6">
         <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>41</v>
@@ -8826,7 +8790,7 @@
         <v>90</v>
       </c>
       <c r="E48" s="62" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F48" s="62" t="s">
         <v>60</v>
@@ -8844,301 +8808,323 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="15" t="s">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B49" s="6">
+        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
+        <v>3</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E49" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="F49" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="G49" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H49" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="I49" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="J49" s="56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B50" s="6">
+        <f xml:space="preserve"> ROW( co_scalarInfo[[#This Row],[row_id]] ) - ROW( co_scalarInfo[[#Headers],[row_id]] )</f>
+        <v>4</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E50" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="F50" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="G50" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="H50" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="I50" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="J50" s="56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
-      <c r="P51" s="15"/>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="15"/>
-      <c r="S51" s="15"/>
-      <c r="T51" s="15"/>
-      <c r="U51" s="15"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B53" s="24" t="s">
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="15"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
+      <c r="S53" s="15"/>
+      <c r="T53" s="15"/>
+      <c r="U53" s="15"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B55" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="24" t="s">
+      <c r="C55" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="D53" s="24" t="s">
+      <c r="D55" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="E53" s="25" t="s">
+      <c r="E55" s="25" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B54" s="4">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B56" s="4">
         <f xml:space="preserve"> ROW( co_econMultipliers[[#This Row],[row_id]] ) - ROW( co_econMultipliers[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D54" s="38" t="s">
+      <c r="D56" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E54" s="39" t="s">
+      <c r="E56" s="39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="15" t="s">
+    <row r="60" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="15"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
-      <c r="P58" s="15"/>
-      <c r="Q58" s="15"/>
-      <c r="R58" s="15"/>
-      <c r="S58" s="15"/>
-      <c r="T58" s="15"/>
-      <c r="U58" s="15"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B60" s="31" t="s">
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="15"/>
+      <c r="R60" s="15"/>
+      <c r="S60" s="15"/>
+      <c r="T60" s="15"/>
+      <c r="U60" s="15"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B62" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C62" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D62" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="E60" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="F60" s="33" t="s">
+      <c r="E62" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="F62" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="G60" s="32" t="s">
+      <c r="G62" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="H60" s="32" t="s">
+      <c r="H62" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="I60" s="30" t="s">
+      <c r="I62" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="J60" s="30" t="s">
+      <c r="J62" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="K60" s="30" t="s">
+      <c r="K62" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="L60" s="30" t="s">
+      <c r="L62" s="30" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B61" s="4">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B63" s="4">
         <f xml:space="preserve"> ROW( co_modelTypes[[#This Row],[row_id]] ) - ROW( co_modelTypes[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C63" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D63" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E61" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="F61" s="35" t="s">
+      <c r="E63" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="F63" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="G61" s="34" t="s">
+      <c r="G63" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="H61" s="34" t="s">
+      <c r="H63" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="I61" s="36">
+      <c r="I63" s="36">
         <v>1</v>
       </c>
-      <c r="J61" s="36">
+      <c r="J63" s="36">
         <v>1995</v>
       </c>
-      <c r="K61" s="36">
+      <c r="K63" s="36">
         <v>6</v>
       </c>
-      <c r="L61" s="36">
+      <c r="L63" s="36">
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="15"/>
-      <c r="P64" s="15"/>
-      <c r="Q64" s="15"/>
-      <c r="R64" s="15"/>
-      <c r="S64" s="15"/>
-      <c r="T64" s="15"/>
-      <c r="U64" s="15"/>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B66" s="37" t="s">
+    <row r="66" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
+      <c r="R66" s="15"/>
+      <c r="S66" s="15"/>
+      <c r="T66" s="15"/>
+      <c r="U66" s="15"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B68" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="24" t="s">
+      <c r="C68" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="D66" s="24" t="s">
-        <v>336</v>
-      </c>
-      <c r="E66" s="24" t="s">
+      <c r="D68" s="24" t="s">
+        <v>337</v>
+      </c>
+      <c r="E68" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="F66" s="25" t="s">
+      <c r="F68" s="25" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B67" s="4">
-        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>1</v>
-      </c>
-      <c r="C67" s="67" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>CanESM2</v>
-      </c>
-      <c r="D67" s="38">
-        <v>6</v>
-      </c>
-      <c r="E67" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="F67" s="65" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B68" s="4">
-        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>2</v>
-      </c>
-      <c r="C68" s="67" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>CCSM4</v>
-      </c>
-      <c r="D68" s="38">
-        <v>5</v>
-      </c>
-      <c r="E68" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="F68" s="65" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B69" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C69" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>GISSE2R</v>
+        <v>CanESM2</v>
       </c>
       <c r="D69" s="38">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E69" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F69" s="65" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B70" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C70" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>HadGEM2ES</v>
+        <v>CCSM4</v>
       </c>
       <c r="D70" s="38">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E70" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F70" s="65" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B71" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C71" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>MIROC5</v>
+        <v>GISSE2R</v>
       </c>
       <c r="D71" s="38">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E71" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F71" s="65" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B72" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C72" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>GFDLCM3</v>
+        <v>HadGEM2ES</v>
       </c>
       <c r="D72" s="38">
         <v>6</v>
@@ -9147,1216 +9133,1255 @@
         <v>72</v>
       </c>
       <c r="F72" s="65" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B73" s="4">
         <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C73" s="67" t="str">
         <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
-        <v>MRICGCM3</v>
+        <v>MIROC5</v>
       </c>
       <c r="D73" s="38">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E73" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F73" s="65" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C76" s="15"/>
-      <c r="D76" s="15"/>
-      <c r="E76" s="15"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
-      <c r="H76" s="15"/>
-      <c r="I76" s="15"/>
-      <c r="J76" s="15"/>
-      <c r="K76" s="15"/>
-      <c r="L76" s="15"/>
-      <c r="M76" s="15"/>
-      <c r="N76" s="15"/>
-      <c r="O76" s="15"/>
-      <c r="P76" s="15"/>
-      <c r="Q76" s="15"/>
-      <c r="R76" s="15"/>
-      <c r="S76" s="15"/>
-      <c r="T76" s="15"/>
-      <c r="U76" s="15"/>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B78" s="24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B74" s="4">
+        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
+        <v>6</v>
+      </c>
+      <c r="C74" s="67" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
+        <v>GFDLCM3</v>
+      </c>
+      <c r="D74" s="38">
+        <v>6</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F74" s="65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B75" s="4">
+        <f xml:space="preserve"> ROW( co_models[[#This Row],[row_id]] ) - ROW( co_models[[#Headers],[row_id]] )</f>
+        <v>7</v>
+      </c>
+      <c r="C75" s="67" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( SUBSTITUTE( co_models[[#This Row],[model_label]], " ", "" ), "-", "" )</f>
+        <v>MRICGCM3</v>
+      </c>
+      <c r="D75" s="38">
+        <v>3</v>
+      </c>
+      <c r="E75" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F75" s="65" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C78" s="15"/>
+      <c r="D78" s="15"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+      <c r="T78" s="15"/>
+      <c r="U78" s="15"/>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B80" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C78" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="D78" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="E78" s="24" t="s">
+      <c r="C80" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D80" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F80" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="F78" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="G78" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="H78" s="26" t="s">
+      <c r="G80" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="I78" s="26" t="s">
+      <c r="H80" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="J78" s="26" t="s">
+      <c r="I80" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="J80" s="26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B79" s="4">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B81" s="4">
         <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C79" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D79" s="38" t="s">
+      <c r="C81" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D81" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="E79" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="F79" s="22" t="s">
+      <c r="E81" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="F81" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="G79" s="22">
+      <c r="G81" s="22">
         <v>0</v>
       </c>
-      <c r="H79" s="22"/>
-      <c r="I79" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="J79" s="22">
+      <c r="H81" s="22"/>
+      <c r="I81" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="J81" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B80" s="4">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B82" s="4">
         <f xml:space="preserve"> ROW( co_inputInfo[[#This Row],[row_id]] ) - ROW( co_inputInfo[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C82" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D80" s="38" t="s">
+      <c r="D82" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="E80" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="F80" s="22" t="s">
+      <c r="E82" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="F82" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="G80" s="22">
+      <c r="G82" s="22">
         <v>0</v>
       </c>
-      <c r="H80" s="22"/>
-      <c r="I80" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="J80" s="22">
+      <c r="H82" s="22"/>
+      <c r="I82" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="J82" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
-      <c r="B83" s="15" t="s">
+    <row r="85" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="14"/>
+      <c r="B85" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C83" s="15"/>
-      <c r="D83" s="15"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="15"/>
-      <c r="J83" s="15"/>
-      <c r="K83" s="15"/>
-      <c r="L83" s="15"/>
-      <c r="M83" s="15"/>
-      <c r="N83" s="15"/>
-      <c r="O83" s="15"/>
-      <c r="P83" s="15"/>
-      <c r="Q83" s="15"/>
-      <c r="R83" s="15"/>
-      <c r="S83" s="15"/>
-      <c r="T83" s="15"/>
-      <c r="U83" s="15"/>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B85" s="37" t="s">
+      <c r="C85" s="15"/>
+      <c r="D85" s="15"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15"/>
+      <c r="S85" s="15"/>
+      <c r="T85" s="15"/>
+      <c r="U85" s="15"/>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B87" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C85" s="24" t="s">
+      <c r="C87" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D85" s="25" t="s">
-        <v>340</v>
-      </c>
-      <c r="E85" s="2"/>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B86" s="4">
-        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>1</v>
-      </c>
-      <c r="C86" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="25" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Midwest</v>
-      </c>
-      <c r="E86" s="2"/>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B87" s="4">
-        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>2</v>
-      </c>
-      <c r="C87" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" s="25" t="str">
-        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Northeast</v>
+      <c r="D87" s="25" t="s">
+        <v>342</v>
       </c>
       <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B88" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C88" s="38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D88" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>NorthernPlains</v>
+        <v>Midwest</v>
       </c>
       <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B89" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C89" s="38" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D89" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Northwest</v>
+        <v>Northeast</v>
       </c>
       <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B90" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C90" s="38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D90" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>Southeast</v>
+        <v>NorthernPlains</v>
       </c>
       <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B91" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D91" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
-        <v>SouthernPlains</v>
+        <v>Northwest</v>
       </c>
       <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B92" s="4">
         <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C92" s="38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D92" s="25" t="str">
         <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
+        <v>Southeast</v>
+      </c>
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B93" s="4">
+        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
+        <v>6</v>
+      </c>
+      <c r="C93" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="25" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
+        <v>SouthernPlains</v>
+      </c>
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B94" s="4">
+        <f xml:space="preserve"> ROW( co_regions[[#This Row],[row_id]] ) - ROW( co_regions[[#Headers],[row_id]] )</f>
+        <v>7</v>
+      </c>
+      <c r="C94" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D94" s="25" t="str">
+        <f xml:space="preserve"> SUBSTITUTE( co_regions[[#This Row],[region_label]], " ", "" )</f>
         <v>Southwest</v>
       </c>
-      <c r="E92" s="2"/>
-    </row>
-    <row r="95" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
-      <c r="B95" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="C95" s="15"/>
-      <c r="D95" s="15"/>
-      <c r="E95" s="15"/>
-      <c r="F95" s="15"/>
-      <c r="G95" s="15"/>
-      <c r="H95" s="15"/>
-      <c r="I95" s="15"/>
-      <c r="J95" s="15"/>
-      <c r="K95" s="15"/>
-      <c r="L95" s="15"/>
-      <c r="M95" s="15"/>
-      <c r="N95" s="15"/>
-      <c r="O95" s="15"/>
-      <c r="P95" s="15"/>
-      <c r="Q95" s="15"/>
-      <c r="R95" s="15"/>
-      <c r="S95" s="15"/>
-      <c r="T95" s="15"/>
-      <c r="U95" s="15"/>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B97" s="2" t="s">
+      <c r="E94" s="2"/>
+    </row>
+    <row r="97" spans="1:21" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="14"/>
+      <c r="B97" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C97" s="15"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
+      <c r="J97" s="15"/>
+      <c r="K97" s="15"/>
+      <c r="L97" s="15"/>
+      <c r="M97" s="15"/>
+      <c r="N97" s="15"/>
+      <c r="O97" s="15"/>
+      <c r="P97" s="15"/>
+      <c r="Q97" s="15"/>
+      <c r="R97" s="15"/>
+      <c r="S97" s="15"/>
+      <c r="T97" s="15"/>
+      <c r="U97" s="15"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B99" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D97" s="2" t="s">
+      <c r="C99" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="E97" s="2" t="s">
+      <c r="D99" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F97" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B98" s="2">
+      <c r="F99" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B100" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>1</v>
       </c>
-      <c r="C98" s="63" t="s">
-        <v>236</v>
-      </c>
-      <c r="D98" s="63" t="s">
+      <c r="C100" s="63" t="s">
         <v>237</v>
       </c>
-      <c r="E98" s="63" t="s">
+      <c r="D100" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="E100" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="F98" s="64">
+      <c r="F100" s="64">
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B99" s="2">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B101" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>2</v>
       </c>
-      <c r="C99" s="63" t="s">
-        <v>238</v>
-      </c>
-      <c r="D99" s="63" t="s">
+      <c r="C101" s="63" t="s">
         <v>239</v>
       </c>
-      <c r="E99" s="63" t="s">
+      <c r="D101" s="63" t="s">
+        <v>240</v>
+      </c>
+      <c r="E101" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="F99" s="64">
+      <c r="F101" s="64">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B100" s="2">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B102" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>3</v>
       </c>
-      <c r="C100" s="63" t="s">
-        <v>240</v>
-      </c>
-      <c r="D100" s="63" t="s">
+      <c r="C102" s="63" t="s">
         <v>241</v>
       </c>
-      <c r="E100" s="63" t="s">
+      <c r="D102" s="63" t="s">
+        <v>242</v>
+      </c>
+      <c r="E102" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="F100" s="64">
+      <c r="F102" s="64">
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B101" s="2">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B103" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>4</v>
       </c>
-      <c r="C101" s="63" t="s">
-        <v>242</v>
-      </c>
-      <c r="D101" s="63" t="s">
+      <c r="C103" s="63" t="s">
         <v>243</v>
       </c>
-      <c r="E101" s="63" t="s">
+      <c r="D103" s="63" t="s">
+        <v>244</v>
+      </c>
+      <c r="E103" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="F101" s="64">
+      <c r="F103" s="64">
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B102" s="2">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B104" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>5</v>
       </c>
-      <c r="C102" s="63" t="s">
-        <v>244</v>
-      </c>
-      <c r="D102" s="63" t="s">
+      <c r="C104" s="63" t="s">
         <v>245</v>
       </c>
-      <c r="E102" s="63" t="s">
+      <c r="D104" s="63" t="s">
+        <v>246</v>
+      </c>
+      <c r="E104" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="F102" s="64">
+      <c r="F104" s="64">
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B103" s="2">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B105" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>6</v>
       </c>
-      <c r="C103" s="63" t="s">
-        <v>246</v>
-      </c>
-      <c r="D103" s="63" t="s">
+      <c r="C105" s="63" t="s">
         <v>247</v>
       </c>
-      <c r="E103" s="63" t="s">
+      <c r="D105" s="63" t="s">
+        <v>248</v>
+      </c>
+      <c r="E105" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="F103" s="64">
+      <c r="F105" s="64">
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B104" s="2">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B106" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>7</v>
       </c>
-      <c r="C104" s="63" t="s">
-        <v>248</v>
-      </c>
-      <c r="D104" s="63" t="s">
+      <c r="C106" s="63" t="s">
         <v>249</v>
       </c>
-      <c r="E104" s="63" t="s">
+      <c r="D106" s="63" t="s">
+        <v>250</v>
+      </c>
+      <c r="E106" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="F104" s="64">
+      <c r="F106" s="64">
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B105" s="2">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B107" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>8</v>
       </c>
-      <c r="C105" s="63" t="s">
-        <v>250</v>
-      </c>
-      <c r="D105" s="63" t="s">
+      <c r="C107" s="63" t="s">
         <v>251</v>
       </c>
-      <c r="E105" s="63" t="s">
+      <c r="D107" s="63" t="s">
+        <v>252</v>
+      </c>
+      <c r="E107" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="F105" s="64">
+      <c r="F107" s="64">
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B106" s="2">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B108" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>9</v>
       </c>
-      <c r="C106" s="63" t="s">
-        <v>252</v>
-      </c>
-      <c r="D106" s="63" t="s">
+      <c r="C108" s="63" t="s">
         <v>253</v>
       </c>
-      <c r="E106" s="63" t="s">
+      <c r="D108" s="63" t="s">
+        <v>254</v>
+      </c>
+      <c r="E108" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="F106" s="64">
+      <c r="F108" s="64">
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B107" s="2">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B109" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>10</v>
       </c>
-      <c r="C107" s="63" t="s">
-        <v>254</v>
-      </c>
-      <c r="D107" s="63" t="s">
+      <c r="C109" s="63" t="s">
         <v>255</v>
       </c>
-      <c r="E107" s="63" t="s">
+      <c r="D109" s="63" t="s">
+        <v>256</v>
+      </c>
+      <c r="E109" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="F107" s="64">
+      <c r="F109" s="64">
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B108" s="2">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B110" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>11</v>
       </c>
-      <c r="C108" s="63" t="s">
-        <v>256</v>
-      </c>
-      <c r="D108" s="63" t="s">
+      <c r="C110" s="63" t="s">
+        <v>257</v>
+      </c>
+      <c r="D110" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="E108" s="63" t="s">
+      <c r="E110" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="F108" s="64">
+      <c r="F110" s="64">
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B109" s="2">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B111" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>12</v>
       </c>
-      <c r="C109" s="63" t="s">
-        <v>257</v>
-      </c>
-      <c r="D109" s="63" t="s">
+      <c r="C111" s="63" t="s">
         <v>258</v>
       </c>
-      <c r="E109" s="63" t="s">
+      <c r="D111" s="63" t="s">
+        <v>259</v>
+      </c>
+      <c r="E111" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="F109" s="64">
+      <c r="F111" s="64">
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B110" s="2">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B112" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>13</v>
       </c>
-      <c r="C110" s="63" t="s">
-        <v>259</v>
-      </c>
-      <c r="D110" s="63" t="s">
+      <c r="C112" s="63" t="s">
         <v>260</v>
       </c>
-      <c r="E110" s="63" t="s">
+      <c r="D112" s="63" t="s">
+        <v>261</v>
+      </c>
+      <c r="E112" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="F110" s="64">
+      <c r="F112" s="64">
         <v>18</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B111" s="2">
-        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>14</v>
-      </c>
-      <c r="C111" s="63" t="s">
-        <v>261</v>
-      </c>
-      <c r="D111" s="63" t="s">
-        <v>262</v>
-      </c>
-      <c r="E111" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="F111" s="64">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B112" s="2">
-        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>15</v>
-      </c>
-      <c r="C112" s="63" t="s">
-        <v>263</v>
-      </c>
-      <c r="D112" s="63" t="s">
-        <v>264</v>
-      </c>
-      <c r="E112" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="F112" s="64">
-        <v>20</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B113" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C113" s="63" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D113" s="63" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E113" s="63" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F113" s="64">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B114" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C114" s="63" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D114" s="63" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E114" s="63" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F114" s="64">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B115" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C115" s="63" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D115" s="63" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E115" s="63" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F115" s="64">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B116" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C116" s="63" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D116" s="63" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E116" s="63" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F116" s="64">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B117" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C117" s="63" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D117" s="63" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E117" s="63" t="s">
         <v>7</v>
       </c>
       <c r="F117" s="64">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B118" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C118" s="63" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D118" s="63" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="E118" s="63" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F118" s="64">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B119" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C119" s="63" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D119" s="63" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E119" s="63" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F119" s="64">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B120" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C120" s="63" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D120" s="63" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E120" s="63" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F120" s="64">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B121" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C121" s="63" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D121" s="63" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E121" s="63" t="s">
         <v>6</v>
       </c>
       <c r="F121" s="64">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B122" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C122" s="63" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D122" s="63" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E122" s="63" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F122" s="64">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B123" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C123" s="63" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D123" s="63" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E123" s="63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F123" s="64">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B124" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C124" s="63" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D124" s="63" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E124" s="63" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F124" s="64">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B125" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C125" s="63" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D125" s="63" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E125" s="63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F125" s="64">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B126" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C126" s="63" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D126" s="63" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E126" s="63" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F126" s="64">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B127" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C127" s="63" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D127" s="63" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E127" s="63" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F127" s="64">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B128" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C128" s="63" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D128" s="63" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E128" s="63" t="s">
         <v>7</v>
       </c>
       <c r="F128" s="64">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="129" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B129" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C129" s="63" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D129" s="63" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E129" s="63" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F129" s="64">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B130" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C130" s="63" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D130" s="63" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E130" s="63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F130" s="64">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B131" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C131" s="63" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D131" s="63" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E131" s="63" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F131" s="64">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B132" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C132" s="63" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D132" s="63" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E132" s="63" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F132" s="64">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B133" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C133" s="63" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D133" s="63" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E133" s="63" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F133" s="64">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B134" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C134" s="63" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D134" s="63" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E134" s="63" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F134" s="64">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B135" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C135" s="63" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D135" s="63" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E135" s="63" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F135" s="64">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B136" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C136" s="63" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D136" s="63" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E136" s="63" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F136" s="64">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B137" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C137" s="63" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D137" s="63" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E137" s="63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F137" s="64">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B138" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C138" s="63" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D138" s="63" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="E138" s="63" t="s">
         <v>10</v>
       </c>
       <c r="F138" s="64">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B139" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C139" s="63" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D139" s="63" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E139" s="63" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F139" s="64">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B140" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C140" s="63" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D140" s="63" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E140" s="63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F140" s="64">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B141" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C141" s="63" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D141" s="63" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E141" s="63" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F141" s="64">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B142" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C142" s="63" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D142" s="63" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E142" s="63" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F142" s="64">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="143" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B143" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C143" s="63" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D143" s="63" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E143" s="63" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F143" s="64">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B144" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C144" s="63" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D144" s="63" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E144" s="63" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F144" s="64">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="145" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B145" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C145" s="63" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D145" s="63" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E145" s="63" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F145" s="64">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B146" s="2">
         <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
+        <v>47</v>
+      </c>
+      <c r="C146" s="63" t="s">
+        <v>328</v>
+      </c>
+      <c r="D146" s="63" t="s">
+        <v>329</v>
+      </c>
+      <c r="E146" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="F146" s="64">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B147" s="2">
+        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
+        <v>48</v>
+      </c>
+      <c r="C147" s="63" t="s">
+        <v>330</v>
+      </c>
+      <c r="D147" s="63" t="s">
+        <v>331</v>
+      </c>
+      <c r="E147" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="F147" s="64">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B148" s="2">
+        <f xml:space="preserve"> ROW( co_states[[#This Row],[row_id]] ) - ROW( co_states[[#Headers],[row_id]] )</f>
         <v>49</v>
       </c>
-      <c r="C146" s="63" t="s">
-        <v>331</v>
-      </c>
-      <c r="D146" s="63" t="s">
+      <c r="C148" s="63" t="s">
         <v>332</v>
       </c>
-      <c r="E146" s="63" t="s">
+      <c r="D148" s="63" t="s">
+        <v>333</v>
+      </c>
+      <c r="E148" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="F146" s="64">
+      <c r="F148" s="64">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="B19:F19">
+  <conditionalFormatting sqref="B21:F21">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula xml:space="preserve"> IF( $E19 = 1, 1, 0)</formula>
+      <formula xml:space="preserve"> IF( $E21 = 1, 1, 0)</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C9" location="loc_coModels" display="loc_coModels" xr:uid="{1AB1FA05-ED11-4F07-8B38-FA24CC6D4F4F}"/>
-    <hyperlink ref="C8" location="loc_coModelTypes" display="loc_coModelTypes" xr:uid="{DCB9BCCC-30A5-4252-A90A-CD0112FF06A8}"/>
+    <hyperlink ref="C8" location="loc_coConstants" display="loc_coConstants" xr:uid="{CFEFD72E-F9ED-4608-B7DD-AFDCEAF6F41D}"/>
+    <hyperlink ref="C10" location="loc_coModels" display="loc_coModels" xr:uid="{1AB1FA05-ED11-4F07-8B38-FA24CC6D4F4F}"/>
+    <hyperlink ref="C9" location="loc_coModelTypes" display="loc_coModelTypes" xr:uid="{DCB9BCCC-30A5-4252-A90A-CD0112FF06A8}"/>
     <hyperlink ref="C6" location="loc_coScalars" display="loc_coScalars" xr:uid="{9B32F273-E2BC-47BF-A60E-7A67D15D4D38}"/>
     <hyperlink ref="C7" location="loc_econMultipliers" display="loc_econMultipliers" xr:uid="{718FB73A-562F-40A4-9DCC-F7B32D89CA2B}"/>
     <hyperlink ref="C2" location="loc_coSectors" display="loc_coSectors" xr:uid="{0561FE55-51F9-468F-AA02-79E8761039B2}"/>
-    <hyperlink ref="C10" location="loc_coRegions" display="loc_coRegions" xr:uid="{A2DFA603-87D5-4136-9543-B92064985F7D}"/>
+    <hyperlink ref="C11" location="loc_coRegions" display="loc_coRegions" xr:uid="{A2DFA603-87D5-4136-9543-B92064985F7D}"/>
     <hyperlink ref="C3" location="loc_coImpactYears" display="loc_coImpactYears" xr:uid="{64F94EF8-131F-4A43-BC1A-C2AA36072515}"/>
     <hyperlink ref="C5" location="loc_coImpactTypes" display="loc_coImpactTypes" xr:uid="{114E9DA3-56F7-4D1E-B736-84EC6F366C11}"/>
     <hyperlink ref="C4" location="loc_coAdaptations" display="loc_coAdaptations" xr:uid="{7F53C6E9-E95F-4F38-8BCD-343D7DB6286E}"/>
-    <hyperlink ref="C11" location="loc_coInputScenarioInfo" display="loc_coInputScenarioInfo" xr:uid="{DA18E986-20B5-4E54-BA62-B58518D13EF3}"/>
-    <hyperlink ref="C12" location="loc_coStates" display="loc_coStates" xr:uid="{8BF3847D-2A5D-4A55-BC5A-0B347ED52535}"/>
+    <hyperlink ref="C12" location="loc_coInputScenarioInfo" display="loc_coInputScenarioInfo" xr:uid="{DA18E986-20B5-4E54-BA62-B58518D13EF3}"/>
+    <hyperlink ref="C13" location="loc_coStates" display="loc_coStates" xr:uid="{8BF3847D-2A5D-4A55-BC5A-0B347ED52535}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -10397,7 +10422,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -10408,13 +10433,13 @@
         <v>22</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F3" s="53" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="75" x14ac:dyDescent="0.25">
@@ -10432,7 +10457,7 @@
         <v>55</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="45" x14ac:dyDescent="0.25">
@@ -10450,12 +10475,12 @@
         <v>55</v>
       </c>
       <c r="F5" s="55" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -10466,10 +10491,10 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -10609,10 +10634,10 @@
         <v>29</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -10624,10 +10649,10 @@
         <v>33</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -10639,10 +10664,10 @@
         <v>87</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -10651,13 +10676,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E6" s="41" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10666,13 +10691,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -10684,10 +10709,10 @@
         <v>77</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E8" s="41" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10699,10 +10724,10 @@
         <v>78</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E9" s="41" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
@@ -10714,10 +10739,10 @@
         <v>79</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -10729,10 +10754,10 @@
         <v>32</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -10744,10 +10769,10 @@
         <v>129</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10759,10 +10784,10 @@
         <v>93</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -10774,10 +10799,10 @@
         <v>130</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -10786,13 +10811,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -10801,13 +10826,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10816,13 +10841,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E17" s="41" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -10831,13 +10856,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -10846,13 +10871,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -10861,13 +10886,13 @@
         <v>17</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -10876,13 +10901,13 @@
         <v>18</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="22.5" x14ac:dyDescent="0.25">
@@ -10891,13 +10916,13 @@
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>